<commit_message>
added notes re leftovers from last year
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lg\repos\leonardguy\dunedin-zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A4C33A-B566-4A0B-9FA0-4BEB928C8F02}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B228C24-CD9D-4B95-908B-6696171C84AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" activeTab="1" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" activeTab="4" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
   </bookViews>
   <sheets>
     <sheet name="numbers" sheetId="5" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="463">
   <si>
     <t>g</t>
   </si>
@@ -1628,6 +1628,15 @@
   </si>
   <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>7x 400g tins left over from last year</t>
+  </si>
+  <si>
+    <t>18x 380g tins left over from last year</t>
+  </si>
+  <si>
+    <t>2x 50g packets left over from last year</t>
   </si>
 </sst>
 </file>
@@ -2461,17 +2470,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4960,7 +4969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604D8F90-B49A-4F27-A51C-C9DAC7C45CC5}">
   <dimension ref="A1:AD428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K190" sqref="K190"/>
     </sheetView>
   </sheetViews>
@@ -8122,12 +8131,12 @@
       <c r="G54" s="100"/>
     </row>
     <row r="55" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="121" t="s">
+      <c r="A55" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="121"/>
-      <c r="C55" s="121"/>
-      <c r="D55" s="121"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
       <c r="E55" s="39" t="s">
         <v>53</v>
       </c>
@@ -15920,10 +15929,10 @@
       </c>
     </row>
     <row r="205" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="118"/>
-      <c r="B205" s="118"/>
-      <c r="C205" s="118"/>
-      <c r="D205" s="118"/>
+      <c r="A205" s="119"/>
+      <c r="B205" s="119"/>
+      <c r="C205" s="119"/>
+      <c r="D205" s="119"/>
       <c r="E205" s="63" t="s">
         <v>352</v>
       </c>
@@ -16227,10 +16236,10 @@
       </c>
     </row>
     <row r="210" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="118"/>
-      <c r="B210" s="118"/>
-      <c r="C210" s="118"/>
-      <c r="D210" s="118"/>
+      <c r="A210" s="119"/>
+      <c r="B210" s="119"/>
+      <c r="C210" s="119"/>
+      <c r="D210" s="119"/>
       <c r="E210" s="39"/>
       <c r="F210" s="39"/>
       <c r="G210" s="44"/>
@@ -16291,10 +16300,10 @@
       <c r="AD211" s="71"/>
     </row>
     <row r="212" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="118"/>
-      <c r="B212" s="118"/>
-      <c r="C212" s="118"/>
-      <c r="D212" s="118"/>
+      <c r="A212" s="119"/>
+      <c r="B212" s="119"/>
+      <c r="C212" s="119"/>
+      <c r="D212" s="119"/>
       <c r="E212" s="39"/>
       <c r="F212" s="39"/>
       <c r="G212" s="44"/>
@@ -16355,10 +16364,10 @@
       <c r="AD213" s="71"/>
     </row>
     <row r="214" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="118"/>
-      <c r="B214" s="118"/>
-      <c r="C214" s="118"/>
-      <c r="D214" s="118"/>
+      <c r="A214" s="119"/>
+      <c r="B214" s="119"/>
+      <c r="C214" s="119"/>
+      <c r="D214" s="119"/>
       <c r="E214" s="39"/>
       <c r="F214" s="39"/>
       <c r="G214" s="44"/>
@@ -16697,10 +16706,10 @@
       </c>
     </row>
     <row r="219" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="118"/>
-      <c r="B219" s="118"/>
-      <c r="C219" s="118"/>
-      <c r="D219" s="118"/>
+      <c r="A219" s="119"/>
+      <c r="B219" s="119"/>
+      <c r="C219" s="119"/>
+      <c r="D219" s="119"/>
       <c r="E219" s="39"/>
       <c r="F219" s="39"/>
       <c r="G219" s="44"/>
@@ -19975,12 +19984,12 @@
       <c r="Z289" s="46"/>
     </row>
     <row r="290" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A290" s="119" t="s">
+      <c r="A290" s="121" t="s">
         <v>276</v>
       </c>
-      <c r="B290" s="119"/>
-      <c r="C290" s="119"/>
-      <c r="D290" s="119"/>
+      <c r="B290" s="121"/>
+      <c r="C290" s="121"/>
+      <c r="D290" s="121"/>
       <c r="E290" s="64"/>
       <c r="F290" s="64"/>
       <c r="G290" s="64"/>
@@ -20709,12 +20718,12 @@
       <c r="AD305" s="71"/>
     </row>
     <row r="306" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A306" s="119" t="s">
+      <c r="A306" s="121" t="s">
         <v>281</v>
       </c>
-      <c r="B306" s="119"/>
-      <c r="C306" s="119"/>
-      <c r="D306" s="119"/>
+      <c r="B306" s="121"/>
+      <c r="C306" s="121"/>
+      <c r="D306" s="121"/>
       <c r="E306" s="40"/>
       <c r="F306" s="57"/>
       <c r="G306" s="57"/>
@@ -23961,10 +23970,10 @@
       </c>
     </row>
     <row r="365" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A365" s="118"/>
-      <c r="B365" s="118"/>
-      <c r="C365" s="118"/>
-      <c r="D365" s="118"/>
+      <c r="A365" s="119"/>
+      <c r="B365" s="119"/>
+      <c r="C365" s="119"/>
+      <c r="D365" s="119"/>
       <c r="E365" s="39"/>
       <c r="F365" s="39"/>
       <c r="G365" s="44"/>
@@ -24214,10 +24223,10 @@
       </c>
     </row>
     <row r="369" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A369" s="118"/>
-      <c r="B369" s="118"/>
-      <c r="C369" s="118"/>
-      <c r="D369" s="118"/>
+      <c r="A369" s="119"/>
+      <c r="B369" s="119"/>
+      <c r="C369" s="119"/>
+      <c r="D369" s="119"/>
       <c r="E369" s="39"/>
       <c r="F369" s="39"/>
       <c r="G369" s="44"/>
@@ -24458,10 +24467,10 @@
       </c>
     </row>
     <row r="373" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A373" s="118"/>
-      <c r="B373" s="118"/>
-      <c r="C373" s="118"/>
-      <c r="D373" s="118"/>
+      <c r="A373" s="119"/>
+      <c r="B373" s="119"/>
+      <c r="C373" s="119"/>
+      <c r="D373" s="119"/>
       <c r="E373" s="39"/>
       <c r="F373" s="39"/>
       <c r="G373" s="44"/>
@@ -24886,10 +24895,10 @@
       </c>
     </row>
     <row r="379" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A379" s="118"/>
-      <c r="B379" s="118"/>
-      <c r="C379" s="118"/>
-      <c r="D379" s="118"/>
+      <c r="A379" s="119"/>
+      <c r="B379" s="119"/>
+      <c r="C379" s="119"/>
+      <c r="D379" s="119"/>
       <c r="E379" s="39"/>
       <c r="F379" s="39"/>
       <c r="G379" s="44"/>
@@ -25310,10 +25319,10 @@
       </c>
     </row>
     <row r="386" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A386" s="118"/>
-      <c r="B386" s="118"/>
-      <c r="C386" s="118"/>
-      <c r="D386" s="118"/>
+      <c r="A386" s="119"/>
+      <c r="B386" s="119"/>
+      <c r="C386" s="119"/>
+      <c r="D386" s="119"/>
       <c r="E386" s="39"/>
       <c r="F386" s="39"/>
       <c r="G386" s="44"/>
@@ -27011,17 +27020,191 @@
     </row>
   </sheetData>
   <mergeCells count="220">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A323:D323"/>
+    <mergeCell ref="A358:D358"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A268:D268"/>
+    <mergeCell ref="A269:D269"/>
+    <mergeCell ref="A271:D271"/>
+    <mergeCell ref="A206:D206"/>
+    <mergeCell ref="A210:D210"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="A288:D288"/>
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A212:D212"/>
+    <mergeCell ref="A213:D213"/>
+    <mergeCell ref="A214:D214"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A391:D391"/>
+    <mergeCell ref="A262:D262"/>
+    <mergeCell ref="A235:D235"/>
+    <mergeCell ref="A202:D202"/>
+    <mergeCell ref="A168:D168"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A317:D317"/>
+    <mergeCell ref="A318:D318"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A224:D224"/>
+    <mergeCell ref="A226:D226"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A388:D388"/>
+    <mergeCell ref="A194:D194"/>
+    <mergeCell ref="A195:D195"/>
+    <mergeCell ref="A215:D215"/>
+    <mergeCell ref="A219:D219"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A319:D319"/>
+    <mergeCell ref="A272:D272"/>
+    <mergeCell ref="A273:D273"/>
+    <mergeCell ref="A274:D274"/>
+    <mergeCell ref="A279:D279"/>
+    <mergeCell ref="A347:D347"/>
+    <mergeCell ref="A353:D353"/>
+    <mergeCell ref="A325:D325"/>
+    <mergeCell ref="A326:D326"/>
+    <mergeCell ref="A280:D280"/>
+    <mergeCell ref="A282:D282"/>
+    <mergeCell ref="A283:D283"/>
+    <mergeCell ref="A309:D309"/>
+    <mergeCell ref="A310:D310"/>
+    <mergeCell ref="A366:D366"/>
+    <mergeCell ref="A316:D316"/>
+    <mergeCell ref="A355:D355"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A159:D159"/>
+    <mergeCell ref="A201:D201"/>
+    <mergeCell ref="A205:D205"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A187:D187"/>
+    <mergeCell ref="A188:D188"/>
+    <mergeCell ref="A192:D192"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A356:D356"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A240:D240"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="A244:D244"/>
+    <mergeCell ref="A246:D246"/>
+    <mergeCell ref="A247:D247"/>
+    <mergeCell ref="A251:D251"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A324:D324"/>
+    <mergeCell ref="A329:D329"/>
+    <mergeCell ref="A339:D339"/>
+    <mergeCell ref="A338:D338"/>
+    <mergeCell ref="A344:D344"/>
+    <mergeCell ref="A290:D290"/>
+    <mergeCell ref="A292:D292"/>
+    <mergeCell ref="A291:D291"/>
+    <mergeCell ref="A295:D295"/>
+    <mergeCell ref="A296:D296"/>
+    <mergeCell ref="A300:D300"/>
+    <mergeCell ref="A301:D301"/>
+    <mergeCell ref="A345:D345"/>
+    <mergeCell ref="A346:D346"/>
+    <mergeCell ref="A387:D387"/>
+    <mergeCell ref="A409:D409"/>
+    <mergeCell ref="A410:D410"/>
+    <mergeCell ref="A415:D415"/>
+    <mergeCell ref="A416:D416"/>
+    <mergeCell ref="A423:D423"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A174:D174"/>
+    <mergeCell ref="A418:D418"/>
+    <mergeCell ref="A354:D354"/>
+    <mergeCell ref="A322:D322"/>
+    <mergeCell ref="A328:D328"/>
+    <mergeCell ref="A303:D303"/>
+    <mergeCell ref="A304:D304"/>
+    <mergeCell ref="A306:D306"/>
+    <mergeCell ref="A305:D305"/>
+    <mergeCell ref="A307:D307"/>
+    <mergeCell ref="A308:D308"/>
+    <mergeCell ref="A357:D357"/>
+    <mergeCell ref="A365:D365"/>
+    <mergeCell ref="A403:D403"/>
+    <mergeCell ref="A404:D404"/>
+    <mergeCell ref="A369:D369"/>
+    <mergeCell ref="A394:D394"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A417:D417"/>
+    <mergeCell ref="A389:D389"/>
+    <mergeCell ref="A286:D286"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A320:D320"/>
+    <mergeCell ref="A321:D321"/>
+    <mergeCell ref="A200:D200"/>
+    <mergeCell ref="A232:D232"/>
+    <mergeCell ref="A233:D233"/>
+    <mergeCell ref="A236:D236"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A259:D259"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A379:D379"/>
+    <mergeCell ref="A380:D380"/>
+    <mergeCell ref="A386:D386"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
@@ -27046,191 +27229,17 @@
     <mergeCell ref="A261:D261"/>
     <mergeCell ref="A393:D393"/>
     <mergeCell ref="A396:D396"/>
-    <mergeCell ref="A394:D394"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A417:D417"/>
-    <mergeCell ref="A389:D389"/>
-    <mergeCell ref="A286:D286"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A320:D320"/>
-    <mergeCell ref="A321:D321"/>
-    <mergeCell ref="A200:D200"/>
-    <mergeCell ref="A232:D232"/>
-    <mergeCell ref="A233:D233"/>
-    <mergeCell ref="A236:D236"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A259:D259"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A379:D379"/>
-    <mergeCell ref="A380:D380"/>
-    <mergeCell ref="A386:D386"/>
-    <mergeCell ref="A387:D387"/>
-    <mergeCell ref="A409:D409"/>
-    <mergeCell ref="A410:D410"/>
-    <mergeCell ref="A415:D415"/>
-    <mergeCell ref="A416:D416"/>
-    <mergeCell ref="A423:D423"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A174:D174"/>
-    <mergeCell ref="A418:D418"/>
-    <mergeCell ref="A354:D354"/>
-    <mergeCell ref="A322:D322"/>
-    <mergeCell ref="A328:D328"/>
-    <mergeCell ref="A303:D303"/>
-    <mergeCell ref="A304:D304"/>
-    <mergeCell ref="A306:D306"/>
-    <mergeCell ref="A305:D305"/>
-    <mergeCell ref="A307:D307"/>
-    <mergeCell ref="A308:D308"/>
-    <mergeCell ref="A357:D357"/>
-    <mergeCell ref="A365:D365"/>
-    <mergeCell ref="A403:D403"/>
-    <mergeCell ref="A404:D404"/>
-    <mergeCell ref="A369:D369"/>
-    <mergeCell ref="A356:D356"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A240:D240"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="A244:D244"/>
-    <mergeCell ref="A246:D246"/>
-    <mergeCell ref="A247:D247"/>
-    <mergeCell ref="A251:D251"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A324:D324"/>
-    <mergeCell ref="A329:D329"/>
-    <mergeCell ref="A339:D339"/>
-    <mergeCell ref="A338:D338"/>
-    <mergeCell ref="A344:D344"/>
-    <mergeCell ref="A290:D290"/>
-    <mergeCell ref="A292:D292"/>
-    <mergeCell ref="A291:D291"/>
-    <mergeCell ref="A295:D295"/>
-    <mergeCell ref="A296:D296"/>
-    <mergeCell ref="A300:D300"/>
-    <mergeCell ref="A301:D301"/>
-    <mergeCell ref="A345:D345"/>
-    <mergeCell ref="A346:D346"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A159:D159"/>
-    <mergeCell ref="A201:D201"/>
-    <mergeCell ref="A205:D205"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="A181:D181"/>
-    <mergeCell ref="A187:D187"/>
-    <mergeCell ref="A188:D188"/>
-    <mergeCell ref="A192:D192"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A388:D388"/>
-    <mergeCell ref="A194:D194"/>
-    <mergeCell ref="A195:D195"/>
-    <mergeCell ref="A215:D215"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A319:D319"/>
-    <mergeCell ref="A272:D272"/>
-    <mergeCell ref="A273:D273"/>
-    <mergeCell ref="A274:D274"/>
-    <mergeCell ref="A279:D279"/>
-    <mergeCell ref="A347:D347"/>
-    <mergeCell ref="A353:D353"/>
-    <mergeCell ref="A325:D325"/>
-    <mergeCell ref="A326:D326"/>
-    <mergeCell ref="A280:D280"/>
-    <mergeCell ref="A282:D282"/>
-    <mergeCell ref="A283:D283"/>
-    <mergeCell ref="A309:D309"/>
-    <mergeCell ref="A310:D310"/>
-    <mergeCell ref="A366:D366"/>
-    <mergeCell ref="A316:D316"/>
-    <mergeCell ref="A355:D355"/>
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A165:D165"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A160:D160"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A391:D391"/>
-    <mergeCell ref="A262:D262"/>
-    <mergeCell ref="A235:D235"/>
-    <mergeCell ref="A202:D202"/>
-    <mergeCell ref="A168:D168"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A317:D317"/>
-    <mergeCell ref="A318:D318"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A224:D224"/>
-    <mergeCell ref="A226:D226"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A289:D289"/>
-    <mergeCell ref="A323:D323"/>
-    <mergeCell ref="A358:D358"/>
-    <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A268:D268"/>
-    <mergeCell ref="A269:D269"/>
-    <mergeCell ref="A271:D271"/>
-    <mergeCell ref="A206:D206"/>
-    <mergeCell ref="A210:D210"/>
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="A288:D288"/>
-    <mergeCell ref="A211:D211"/>
-    <mergeCell ref="A212:D212"/>
-    <mergeCell ref="A213:D213"/>
-    <mergeCell ref="A214:D214"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <conditionalFormatting sqref="M32:T32 M56:T77 M79:T104 M201:T232 M234:T259 M261:T286 M288:T320 M390:T1048576 M48:T48 M53:T54 M14:T14 M29:T29 M322:T355 M143:T165 M357:T388 M167:T199 M16:T23 Q15:T15 M34:T45 M106:T141">
     <cfRule type="cellIs" dxfId="175" priority="269" operator="equal">
@@ -27647,7 +27656,7 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31850,8 +31859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2944F1E-C26E-4F90-A95D-D6E10706BE4A}">
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD68"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31861,7 +31870,7 @@
     <col min="3" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" style="94" customWidth="1"/>
-    <col min="7" max="7" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="94" bestFit="1" customWidth="1"/>
     <col min="9" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -31984,7 +31993,9 @@
         <f>SUMIF(support!C:C,B4,support!L:L)</f>
         <v>1</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>462</v>
+      </c>
       <c r="H4" s="24" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -33253,7 +33264,9 @@
         <f>SUMIF(support!C:C,B46,support!L:L)</f>
         <v>1</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>461</v>
+      </c>
       <c r="H46" s="24" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -33283,7 +33296,9 @@
         <f>SUMIF(support!C:C,B47,support!L:L)</f>
         <v>2</v>
       </c>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>460</v>
+      </c>
       <c r="H47" s="24" t="b">
         <f t="shared" si="1"/>
         <v>0</v>

</xml_diff>

<commit_message>
added lemons to chop list
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lg\repos\leonardguy\dunedin-zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B228C24-CD9D-4B95-908B-6696171C84AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1BF9C-CED5-4946-B15F-2880CB4D0983}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" activeTab="4" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" activeTab="3" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
   </bookViews>
   <sheets>
     <sheet name="numbers" sheetId="5" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="463">
   <si>
     <t>g</t>
   </si>
@@ -2465,22 +2465,22 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4969,8 +4969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604D8F90-B49A-4F27-A51C-C9DAC7C45CC5}">
   <dimension ref="A1:AD428"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K190" sqref="K190"/>
+    <sheetView topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5006,12 +5006,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="102" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>431</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
       <c r="E1" s="40" t="s">
         <v>413</v>
       </c>
@@ -5033,12 +5033,12 @@
       <c r="Z1" s="46"/>
     </row>
     <row r="2" spans="1:30" s="102" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="117" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
       <c r="E2" s="100" t="s">
         <v>53</v>
       </c>
@@ -5114,13 +5114,13 @@
       </c>
     </row>
     <row r="3" spans="1:30" s="102" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="117" t="str">
+      <c r="A3" s="118" t="str">
         <f>_xlfn.CONCAT(F3," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
       <c r="E3" s="100" t="s">
         <v>348</v>
       </c>
@@ -5750,12 +5750,12 @@
       <c r="Z13" s="46"/>
     </row>
     <row r="14" spans="1:30" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="117" t="s">
         <v>429</v>
       </c>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
       <c r="E14" s="40" t="s">
         <v>303</v>
       </c>
@@ -5777,12 +5777,12 @@
       <c r="Z14" s="46"/>
     </row>
     <row r="15" spans="1:30" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="116" t="s">
+      <c r="A15" s="117" t="s">
         <v>430</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
       <c r="E15" s="63" t="s">
         <v>53</v>
       </c>
@@ -5858,13 +5858,13 @@
       </c>
     </row>
     <row r="16" spans="1:30" s="64" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="117" t="str">
+      <c r="A16" s="118" t="str">
         <f>_xlfn.CONCAT(F16," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="63" t="s">
         <v>348</v>
       </c>
@@ -6777,12 +6777,12 @@
       <c r="Z31" s="46"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="116" t="s">
+      <c r="A32" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="116"/>
-      <c r="C32" s="116"/>
-      <c r="D32" s="116"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
       <c r="E32" s="40" t="s">
         <v>184</v>
       </c>
@@ -6790,12 +6790,12 @@
       <c r="G32" s="100"/>
     </row>
     <row r="33" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="117" t="s">
         <v>384</v>
       </c>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="117"/>
       <c r="E33" s="39" t="s">
         <v>53</v>
       </c>
@@ -6871,13 +6871,13 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="117" t="str">
+      <c r="A34" s="118" t="str">
         <f>_xlfn.CONCAT(F34," servings")</f>
         <v>4 servings</v>
       </c>
-      <c r="B34" s="117"/>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
       <c r="E34" s="39" t="s">
         <v>348</v>
       </c>
@@ -8116,12 +8116,12 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="116" t="s">
+      <c r="A54" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="116"/>
-      <c r="C54" s="116"/>
-      <c r="D54" s="116"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="117"/>
+      <c r="D54" s="117"/>
       <c r="E54" s="39" t="s">
         <v>125</v>
       </c>
@@ -8131,12 +8131,12 @@
       <c r="G54" s="100"/>
     </row>
     <row r="55" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="118" t="s">
+      <c r="A55" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="121"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="39" t="s">
         <v>53</v>
       </c>
@@ -8213,13 +8213,13 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="117" t="str">
+      <c r="A56" s="118" t="str">
         <f>_xlfn.CONCAT(F56," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B56" s="117"/>
-      <c r="C56" s="117"/>
-      <c r="D56" s="117"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="118"/>
       <c r="E56" s="63" t="s">
         <v>348</v>
       </c>
@@ -9292,12 +9292,12 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="116" t="s">
+      <c r="A77" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B77" s="116"/>
-      <c r="C77" s="116"/>
-      <c r="D77" s="116"/>
+      <c r="B77" s="117"/>
+      <c r="C77" s="117"/>
+      <c r="D77" s="117"/>
       <c r="E77" s="57" t="s">
         <v>126</v>
       </c>
@@ -9307,12 +9307,12 @@
       <c r="G77" s="100"/>
     </row>
     <row r="78" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A78" s="116" t="s">
+      <c r="A78" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="116"/>
-      <c r="C78" s="116"/>
-      <c r="D78" s="116"/>
+      <c r="B78" s="117"/>
+      <c r="C78" s="117"/>
+      <c r="D78" s="117"/>
       <c r="E78" s="39" t="s">
         <v>53</v>
       </c>
@@ -9387,13 +9387,13 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="117" t="str">
+      <c r="A79" s="118" t="str">
         <f>_xlfn.CONCAT(F79," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B79" s="117"/>
-      <c r="C79" s="117"/>
-      <c r="D79" s="117"/>
+      <c r="B79" s="118"/>
+      <c r="C79" s="118"/>
+      <c r="D79" s="118"/>
       <c r="E79" s="63" t="s">
         <v>348</v>
       </c>
@@ -10703,12 +10703,12 @@
       <c r="P103" s="41"/>
     </row>
     <row r="104" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="116" t="s">
+      <c r="A104" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B104" s="116"/>
-      <c r="C104" s="116"/>
-      <c r="D104" s="116"/>
+      <c r="B104" s="117"/>
+      <c r="C104" s="117"/>
+      <c r="D104" s="117"/>
       <c r="E104" s="40" t="s">
         <v>132</v>
       </c>
@@ -10719,12 +10719,12 @@
       <c r="I104" s="44"/>
     </row>
     <row r="105" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A105" s="116" t="s">
+      <c r="A105" s="117" t="s">
         <v>263</v>
       </c>
-      <c r="B105" s="116"/>
-      <c r="C105" s="116"/>
-      <c r="D105" s="116"/>
+      <c r="B105" s="117"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
       <c r="E105" s="39" t="s">
         <v>53</v>
       </c>
@@ -10801,13 +10801,13 @@
       </c>
     </row>
     <row r="106" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="117" t="str">
+      <c r="A106" s="118" t="str">
         <f>_xlfn.CONCAT(F106," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B106" s="117"/>
-      <c r="C106" s="117"/>
-      <c r="D106" s="117"/>
+      <c r="B106" s="118"/>
+      <c r="C106" s="118"/>
+      <c r="D106" s="118"/>
       <c r="E106" s="63" t="s">
         <v>348</v>
       </c>
@@ -12365,12 +12365,12 @@
       </c>
     </row>
     <row r="141" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="116" t="s">
+      <c r="A141" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B141" s="116"/>
-      <c r="C141" s="116"/>
-      <c r="D141" s="116"/>
+      <c r="B141" s="117"/>
+      <c r="C141" s="117"/>
+      <c r="D141" s="117"/>
       <c r="E141" s="40" t="s">
         <v>127</v>
       </c>
@@ -12381,12 +12381,12 @@
       <c r="H141" s="44"/>
     </row>
     <row r="142" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A142" s="116" t="s">
+      <c r="A142" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B142" s="116"/>
-      <c r="C142" s="116"/>
-      <c r="D142" s="116"/>
+      <c r="B142" s="117"/>
+      <c r="C142" s="117"/>
+      <c r="D142" s="117"/>
       <c r="E142" s="39" t="s">
         <v>53</v>
       </c>
@@ -12463,13 +12463,13 @@
       </c>
     </row>
     <row r="143" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="117" t="str">
+      <c r="A143" s="118" t="str">
         <f>_xlfn.CONCAT(F143," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B143" s="117"/>
-      <c r="C143" s="117"/>
-      <c r="D143" s="117"/>
+      <c r="B143" s="118"/>
+      <c r="C143" s="118"/>
+      <c r="D143" s="118"/>
       <c r="E143" s="63" t="s">
         <v>348</v>
       </c>
@@ -13649,12 +13649,12 @@
       </c>
     </row>
     <row r="165" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="116" t="s">
+      <c r="A165" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="B165" s="116"/>
-      <c r="C165" s="116"/>
-      <c r="D165" s="116"/>
+      <c r="B165" s="117"/>
+      <c r="C165" s="117"/>
+      <c r="D165" s="117"/>
       <c r="E165" s="40" t="s">
         <v>134</v>
       </c>
@@ -13664,12 +13664,12 @@
       <c r="G165" s="100"/>
     </row>
     <row r="166" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A166" s="116" t="s">
+      <c r="A166" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="B166" s="116"/>
-      <c r="C166" s="116"/>
-      <c r="D166" s="116"/>
+      <c r="B166" s="117"/>
+      <c r="C166" s="117"/>
+      <c r="D166" s="117"/>
       <c r="E166" s="39" t="s">
         <v>53</v>
       </c>
@@ -13745,13 +13745,13 @@
       </c>
     </row>
     <row r="167" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="117" t="str">
+      <c r="A167" s="118" t="str">
         <f>_xlfn.CONCAT(F167," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B167" s="117"/>
-      <c r="C167" s="117"/>
-      <c r="D167" s="117"/>
+      <c r="B167" s="118"/>
+      <c r="C167" s="118"/>
+      <c r="D167" s="118"/>
       <c r="E167" s="63" t="s">
         <v>348</v>
       </c>
@@ -15156,11 +15156,11 @@
       </c>
       <c r="V189" s="41" t="b">
         <f>INDEX(itemPrepMethods, MATCH(K189, itemNames, 0))="chop"</f>
-        <v>0</v>
-      </c>
-      <c r="W189" s="54" t="str">
+        <v>1</v>
+      </c>
+      <c r="W189" s="54">
         <f>IF(V189, Q189, "")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="X189" s="55" t="str">
         <f>IF(V189, IF(L189 = "", "", L189), "")</f>
@@ -15168,7 +15168,7 @@
       </c>
       <c r="Y189" s="55" t="str">
         <f>IF(V189, K189, "")</f>
-        <v/>
+        <v>juiced lemons</v>
       </c>
       <c r="Z189" s="56"/>
       <c r="AA189" s="41" t="b">
@@ -15637,12 +15637,12 @@
       </c>
     </row>
     <row r="199" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="116" t="s">
+      <c r="A199" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B199" s="116"/>
-      <c r="C199" s="116"/>
-      <c r="D199" s="116"/>
+      <c r="B199" s="117"/>
+      <c r="C199" s="117"/>
+      <c r="D199" s="117"/>
       <c r="E199" s="40" t="s">
         <v>129</v>
       </c>
@@ -15653,12 +15653,12 @@
       <c r="H199" s="44"/>
     </row>
     <row r="200" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A200" s="116" t="s">
+      <c r="A200" s="117" t="s">
         <v>249</v>
       </c>
-      <c r="B200" s="116"/>
-      <c r="C200" s="116"/>
-      <c r="D200" s="116"/>
+      <c r="B200" s="117"/>
+      <c r="C200" s="117"/>
+      <c r="D200" s="117"/>
       <c r="E200" s="39" t="s">
         <v>53</v>
       </c>
@@ -15735,13 +15735,13 @@
       </c>
     </row>
     <row r="201" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="117" t="str">
+      <c r="A201" s="118" t="str">
         <f>_xlfn.CONCAT(F201," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B201" s="117"/>
-      <c r="C201" s="117"/>
-      <c r="D201" s="117"/>
+      <c r="B201" s="118"/>
+      <c r="C201" s="118"/>
+      <c r="D201" s="118"/>
       <c r="E201" s="63" t="s">
         <v>348</v>
       </c>
@@ -15929,10 +15929,10 @@
       </c>
     </row>
     <row r="205" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="119"/>
-      <c r="B205" s="119"/>
-      <c r="C205" s="119"/>
-      <c r="D205" s="119"/>
+      <c r="A205" s="116"/>
+      <c r="B205" s="116"/>
+      <c r="C205" s="116"/>
+      <c r="D205" s="116"/>
       <c r="E205" s="63" t="s">
         <v>352</v>
       </c>
@@ -16236,10 +16236,10 @@
       </c>
     </row>
     <row r="210" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="119"/>
-      <c r="B210" s="119"/>
-      <c r="C210" s="119"/>
-      <c r="D210" s="119"/>
+      <c r="A210" s="116"/>
+      <c r="B210" s="116"/>
+      <c r="C210" s="116"/>
+      <c r="D210" s="116"/>
       <c r="E210" s="39"/>
       <c r="F210" s="39"/>
       <c r="G210" s="44"/>
@@ -16300,10 +16300,10 @@
       <c r="AD211" s="71"/>
     </row>
     <row r="212" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="119"/>
-      <c r="B212" s="119"/>
-      <c r="C212" s="119"/>
-      <c r="D212" s="119"/>
+      <c r="A212" s="116"/>
+      <c r="B212" s="116"/>
+      <c r="C212" s="116"/>
+      <c r="D212" s="116"/>
       <c r="E212" s="39"/>
       <c r="F212" s="39"/>
       <c r="G212" s="44"/>
@@ -16364,10 +16364,10 @@
       <c r="AD213" s="71"/>
     </row>
     <row r="214" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="119"/>
-      <c r="B214" s="119"/>
-      <c r="C214" s="119"/>
-      <c r="D214" s="119"/>
+      <c r="A214" s="116"/>
+      <c r="B214" s="116"/>
+      <c r="C214" s="116"/>
+      <c r="D214" s="116"/>
       <c r="E214" s="39"/>
       <c r="F214" s="39"/>
       <c r="G214" s="44"/>
@@ -16706,10 +16706,10 @@
       </c>
     </row>
     <row r="219" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="119"/>
-      <c r="B219" s="119"/>
-      <c r="C219" s="119"/>
-      <c r="D219" s="119"/>
+      <c r="A219" s="116"/>
+      <c r="B219" s="116"/>
+      <c r="C219" s="116"/>
+      <c r="D219" s="116"/>
       <c r="E219" s="39"/>
       <c r="F219" s="39"/>
       <c r="G219" s="44"/>
@@ -17228,12 +17228,12 @@
       </c>
     </row>
     <row r="232" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A232" s="116" t="s">
+      <c r="A232" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="B232" s="116"/>
-      <c r="C232" s="116"/>
-      <c r="D232" s="116"/>
+      <c r="B232" s="117"/>
+      <c r="C232" s="117"/>
+      <c r="D232" s="117"/>
       <c r="E232" s="40" t="s">
         <v>130</v>
       </c>
@@ -17244,12 +17244,12 @@
       <c r="H232" s="44"/>
     </row>
     <row r="233" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A233" s="116" t="s">
+      <c r="A233" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="B233" s="116"/>
-      <c r="C233" s="116"/>
-      <c r="D233" s="116"/>
+      <c r="B233" s="117"/>
+      <c r="C233" s="117"/>
+      <c r="D233" s="117"/>
       <c r="E233" s="39" t="s">
         <v>53</v>
       </c>
@@ -17326,13 +17326,13 @@
       </c>
     </row>
     <row r="234" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="117" t="str">
+      <c r="A234" s="118" t="str">
         <f>_xlfn.CONCAT(F234," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B234" s="117"/>
-      <c r="C234" s="117"/>
-      <c r="D234" s="117"/>
+      <c r="B234" s="118"/>
+      <c r="C234" s="118"/>
+      <c r="D234" s="118"/>
       <c r="E234" s="63" t="s">
         <v>348</v>
       </c>
@@ -18687,12 +18687,12 @@
       </c>
     </row>
     <row r="259" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A259" s="116" t="s">
+      <c r="A259" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="B259" s="116"/>
-      <c r="C259" s="116"/>
-      <c r="D259" s="116"/>
+      <c r="B259" s="117"/>
+      <c r="C259" s="117"/>
+      <c r="D259" s="117"/>
       <c r="E259" s="40" t="s">
         <v>131</v>
       </c>
@@ -18703,12 +18703,12 @@
       <c r="H259" s="44"/>
     </row>
     <row r="260" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A260" s="116" t="s">
+      <c r="A260" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="B260" s="116"/>
-      <c r="C260" s="116"/>
-      <c r="D260" s="116"/>
+      <c r="B260" s="117"/>
+      <c r="C260" s="117"/>
+      <c r="D260" s="117"/>
       <c r="E260" s="39" t="s">
         <v>53</v>
       </c>
@@ -18785,13 +18785,13 @@
       </c>
     </row>
     <row r="261" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="117" t="str">
+      <c r="A261" s="118" t="str">
         <f>_xlfn.CONCAT(F261," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B261" s="117"/>
-      <c r="C261" s="117"/>
-      <c r="D261" s="117"/>
+      <c r="B261" s="118"/>
+      <c r="C261" s="118"/>
+      <c r="D261" s="118"/>
       <c r="E261" s="63" t="s">
         <v>348</v>
       </c>
@@ -19841,12 +19841,12 @@
       <c r="AD285" s="64"/>
     </row>
     <row r="286" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A286" s="116" t="s">
+      <c r="A286" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="B286" s="116"/>
-      <c r="C286" s="116"/>
-      <c r="D286" s="116"/>
+      <c r="B286" s="117"/>
+      <c r="C286" s="117"/>
+      <c r="D286" s="117"/>
       <c r="E286" s="39" t="s">
         <v>136</v>
       </c>
@@ -19855,12 +19855,12 @@
       <c r="H286" s="44"/>
     </row>
     <row r="287" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A287" s="116" t="s">
+      <c r="A287" s="117" t="s">
         <v>275</v>
       </c>
-      <c r="B287" s="116"/>
-      <c r="C287" s="116"/>
-      <c r="D287" s="116"/>
+      <c r="B287" s="117"/>
+      <c r="C287" s="117"/>
+      <c r="D287" s="117"/>
       <c r="E287" s="39" t="s">
         <v>53</v>
       </c>
@@ -19937,13 +19937,13 @@
       </c>
     </row>
     <row r="288" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="117" t="str">
+      <c r="A288" s="118" t="str">
         <f>_xlfn.CONCAT(F288," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B288" s="117"/>
-      <c r="C288" s="117"/>
-      <c r="D288" s="117"/>
+      <c r="B288" s="118"/>
+      <c r="C288" s="118"/>
+      <c r="D288" s="118"/>
       <c r="E288" s="63" t="s">
         <v>348</v>
       </c>
@@ -19984,12 +19984,12 @@
       <c r="Z289" s="46"/>
     </row>
     <row r="290" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A290" s="121" t="s">
+      <c r="A290" s="119" t="s">
         <v>276</v>
       </c>
-      <c r="B290" s="121"/>
-      <c r="C290" s="121"/>
-      <c r="D290" s="121"/>
+      <c r="B290" s="119"/>
+      <c r="C290" s="119"/>
+      <c r="D290" s="119"/>
       <c r="E290" s="64"/>
       <c r="F290" s="64"/>
       <c r="G290" s="64"/>
@@ -20718,12 +20718,12 @@
       <c r="AD305" s="71"/>
     </row>
     <row r="306" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A306" s="121" t="s">
+      <c r="A306" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="B306" s="121"/>
-      <c r="C306" s="121"/>
-      <c r="D306" s="121"/>
+      <c r="B306" s="119"/>
+      <c r="C306" s="119"/>
+      <c r="D306" s="119"/>
       <c r="E306" s="40"/>
       <c r="F306" s="57"/>
       <c r="G306" s="57"/>
@@ -21340,12 +21340,12 @@
       <c r="H319" s="44"/>
     </row>
     <row r="320" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A320" s="116" t="s">
+      <c r="A320" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B320" s="116"/>
-      <c r="C320" s="116"/>
-      <c r="D320" s="116"/>
+      <c r="B320" s="117"/>
+      <c r="C320" s="117"/>
+      <c r="D320" s="117"/>
       <c r="E320" s="40" t="s">
         <v>133</v>
       </c>
@@ -21355,12 +21355,12 @@
       <c r="G320" s="100"/>
     </row>
     <row r="321" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A321" s="116" t="s">
+      <c r="A321" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B321" s="116"/>
-      <c r="C321" s="116"/>
-      <c r="D321" s="116"/>
+      <c r="B321" s="117"/>
+      <c r="C321" s="117"/>
+      <c r="D321" s="117"/>
       <c r="E321" s="39" t="s">
         <v>53</v>
       </c>
@@ -21436,13 +21436,13 @@
       </c>
     </row>
     <row r="322" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A322" s="117" t="str">
+      <c r="A322" s="118" t="str">
         <f>_xlfn.CONCAT(F322," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B322" s="117"/>
-      <c r="C322" s="117"/>
-      <c r="D322" s="117"/>
+      <c r="B322" s="118"/>
+      <c r="C322" s="118"/>
+      <c r="D322" s="118"/>
       <c r="E322" s="63" t="s">
         <v>348</v>
       </c>
@@ -23062,11 +23062,11 @@
       </c>
       <c r="V349" s="41" t="b">
         <f>INDEX(itemPrepMethods, MATCH(K349, itemNames, 0))="chop"</f>
-        <v>0</v>
-      </c>
-      <c r="W349" s="54" t="str">
+        <v>1</v>
+      </c>
+      <c r="W349" s="54">
         <f>IF(V349, Q349, "")</f>
-        <v/>
+        <v>1.25</v>
       </c>
       <c r="X349" s="55" t="str">
         <f>IF(V349, IF(L349 = "", "", L349), "")</f>
@@ -23074,7 +23074,7 @@
       </c>
       <c r="Y349" s="55" t="str">
         <f>IF(V349, K349, "")</f>
-        <v/>
+        <v>juiced lemons</v>
       </c>
       <c r="Z349" s="56"/>
       <c r="AA349" s="41" t="b">
@@ -23298,12 +23298,12 @@
       <c r="N354" s="41"/>
     </row>
     <row r="355" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A355" s="116" t="s">
+      <c r="A355" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="B355" s="116"/>
-      <c r="C355" s="116"/>
-      <c r="D355" s="116"/>
+      <c r="B355" s="117"/>
+      <c r="C355" s="117"/>
+      <c r="D355" s="117"/>
       <c r="E355" s="40" t="s">
         <v>128</v>
       </c>
@@ -23314,12 +23314,12 @@
       <c r="H355" s="44"/>
     </row>
     <row r="356" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A356" s="116" t="s">
+      <c r="A356" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="B356" s="116"/>
-      <c r="C356" s="116"/>
-      <c r="D356" s="116"/>
+      <c r="B356" s="117"/>
+      <c r="C356" s="117"/>
+      <c r="D356" s="117"/>
       <c r="E356" s="39" t="s">
         <v>53</v>
       </c>
@@ -23396,13 +23396,13 @@
       </c>
     </row>
     <row r="357" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A357" s="117" t="str">
+      <c r="A357" s="118" t="str">
         <f>_xlfn.CONCAT(F357," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B357" s="117"/>
-      <c r="C357" s="117"/>
-      <c r="D357" s="117"/>
+      <c r="B357" s="118"/>
+      <c r="C357" s="118"/>
+      <c r="D357" s="118"/>
       <c r="E357" s="63" t="s">
         <v>348</v>
       </c>
@@ -23970,10 +23970,10 @@
       </c>
     </row>
     <row r="365" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A365" s="119"/>
-      <c r="B365" s="119"/>
-      <c r="C365" s="119"/>
-      <c r="D365" s="119"/>
+      <c r="A365" s="116"/>
+      <c r="B365" s="116"/>
+      <c r="C365" s="116"/>
+      <c r="D365" s="116"/>
       <c r="E365" s="39"/>
       <c r="F365" s="39"/>
       <c r="G365" s="44"/>
@@ -24223,10 +24223,10 @@
       </c>
     </row>
     <row r="369" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A369" s="119"/>
-      <c r="B369" s="119"/>
-      <c r="C369" s="119"/>
-      <c r="D369" s="119"/>
+      <c r="A369" s="116"/>
+      <c r="B369" s="116"/>
+      <c r="C369" s="116"/>
+      <c r="D369" s="116"/>
       <c r="E369" s="39"/>
       <c r="F369" s="39"/>
       <c r="G369" s="44"/>
@@ -24467,10 +24467,10 @@
       </c>
     </row>
     <row r="373" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A373" s="119"/>
-      <c r="B373" s="119"/>
-      <c r="C373" s="119"/>
-      <c r="D373" s="119"/>
+      <c r="A373" s="116"/>
+      <c r="B373" s="116"/>
+      <c r="C373" s="116"/>
+      <c r="D373" s="116"/>
       <c r="E373" s="39"/>
       <c r="F373" s="39"/>
       <c r="G373" s="44"/>
@@ -24895,10 +24895,10 @@
       </c>
     </row>
     <row r="379" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A379" s="119"/>
-      <c r="B379" s="119"/>
-      <c r="C379" s="119"/>
-      <c r="D379" s="119"/>
+      <c r="A379" s="116"/>
+      <c r="B379" s="116"/>
+      <c r="C379" s="116"/>
+      <c r="D379" s="116"/>
       <c r="E379" s="39"/>
       <c r="F379" s="39"/>
       <c r="G379" s="44"/>
@@ -25319,10 +25319,10 @@
       </c>
     </row>
     <row r="386" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A386" s="119"/>
-      <c r="B386" s="119"/>
-      <c r="C386" s="119"/>
-      <c r="D386" s="119"/>
+      <c r="A386" s="116"/>
+      <c r="B386" s="116"/>
+      <c r="C386" s="116"/>
+      <c r="D386" s="116"/>
       <c r="E386" s="39"/>
       <c r="F386" s="39"/>
       <c r="G386" s="44"/>
@@ -25367,12 +25367,12 @@
       <c r="U387" s="39"/>
     </row>
     <row r="388" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A388" s="116" t="s">
+      <c r="A388" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="B388" s="116"/>
-      <c r="C388" s="116"/>
-      <c r="D388" s="116"/>
+      <c r="B388" s="117"/>
+      <c r="C388" s="117"/>
+      <c r="D388" s="117"/>
       <c r="E388" s="40" t="s">
         <v>135</v>
       </c>
@@ -25382,12 +25382,12 @@
       <c r="G388" s="100"/>
     </row>
     <row r="389" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A389" s="116" t="s">
+      <c r="A389" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="B389" s="116"/>
-      <c r="C389" s="116"/>
-      <c r="D389" s="116"/>
+      <c r="B389" s="117"/>
+      <c r="C389" s="117"/>
+      <c r="D389" s="117"/>
       <c r="E389" s="39" t="s">
         <v>53</v>
       </c>
@@ -25463,13 +25463,13 @@
       </c>
     </row>
     <row r="390" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A390" s="117" t="str">
+      <c r="A390" s="118" t="str">
         <f>_xlfn.CONCAT(F390," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B390" s="117"/>
-      <c r="C390" s="117"/>
-      <c r="D390" s="117"/>
+      <c r="B390" s="118"/>
+      <c r="C390" s="118"/>
+      <c r="D390" s="118"/>
       <c r="E390" s="63" t="s">
         <v>348</v>
       </c>
@@ -26893,12 +26893,12 @@
       <c r="Z416" s="41"/>
     </row>
     <row r="417" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A417" s="116" t="s">
+      <c r="A417" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="B417" s="116"/>
-      <c r="C417" s="116"/>
-      <c r="D417" s="116"/>
+      <c r="B417" s="117"/>
+      <c r="C417" s="117"/>
+      <c r="D417" s="117"/>
       <c r="M417" s="41"/>
       <c r="N417" s="41"/>
       <c r="O417" s="41"/>
@@ -26929,12 +26929,12 @@
       <c r="Z418" s="41"/>
     </row>
     <row r="423" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A423" s="116" t="s">
+      <c r="A423" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="B423" s="116"/>
-      <c r="C423" s="116"/>
-      <c r="D423" s="116"/>
+      <c r="B423" s="117"/>
+      <c r="C423" s="117"/>
+      <c r="D423" s="117"/>
       <c r="M423" s="41"/>
       <c r="N423" s="41"/>
       <c r="O423" s="41"/>
@@ -27020,29 +27020,178 @@
     </row>
   </sheetData>
   <mergeCells count="220">
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A289:D289"/>
-    <mergeCell ref="A323:D323"/>
-    <mergeCell ref="A358:D358"/>
-    <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A268:D268"/>
-    <mergeCell ref="A269:D269"/>
-    <mergeCell ref="A271:D271"/>
-    <mergeCell ref="A206:D206"/>
-    <mergeCell ref="A210:D210"/>
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="A288:D288"/>
-    <mergeCell ref="A211:D211"/>
-    <mergeCell ref="A212:D212"/>
-    <mergeCell ref="A213:D213"/>
-    <mergeCell ref="A214:D214"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="A397:D397"/>
+    <mergeCell ref="A359:D359"/>
+    <mergeCell ref="A390:D390"/>
+    <mergeCell ref="A392:D392"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A203:D203"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A370:D370"/>
+    <mergeCell ref="A373:D373"/>
+    <mergeCell ref="A374:D374"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A261:D261"/>
+    <mergeCell ref="A393:D393"/>
+    <mergeCell ref="A396:D396"/>
+    <mergeCell ref="A394:D394"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A417:D417"/>
+    <mergeCell ref="A389:D389"/>
+    <mergeCell ref="A286:D286"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A320:D320"/>
+    <mergeCell ref="A321:D321"/>
+    <mergeCell ref="A200:D200"/>
+    <mergeCell ref="A232:D232"/>
+    <mergeCell ref="A233:D233"/>
+    <mergeCell ref="A236:D236"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A259:D259"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A379:D379"/>
+    <mergeCell ref="A380:D380"/>
+    <mergeCell ref="A386:D386"/>
+    <mergeCell ref="A387:D387"/>
+    <mergeCell ref="A409:D409"/>
+    <mergeCell ref="A410:D410"/>
+    <mergeCell ref="A415:D415"/>
+    <mergeCell ref="A416:D416"/>
+    <mergeCell ref="A423:D423"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A174:D174"/>
+    <mergeCell ref="A418:D418"/>
+    <mergeCell ref="A354:D354"/>
+    <mergeCell ref="A322:D322"/>
+    <mergeCell ref="A328:D328"/>
+    <mergeCell ref="A303:D303"/>
+    <mergeCell ref="A304:D304"/>
+    <mergeCell ref="A306:D306"/>
+    <mergeCell ref="A305:D305"/>
+    <mergeCell ref="A307:D307"/>
+    <mergeCell ref="A308:D308"/>
+    <mergeCell ref="A357:D357"/>
+    <mergeCell ref="A365:D365"/>
+    <mergeCell ref="A403:D403"/>
+    <mergeCell ref="A404:D404"/>
+    <mergeCell ref="A369:D369"/>
+    <mergeCell ref="A356:D356"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A240:D240"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="A244:D244"/>
+    <mergeCell ref="A246:D246"/>
+    <mergeCell ref="A247:D247"/>
+    <mergeCell ref="A251:D251"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A324:D324"/>
+    <mergeCell ref="A329:D329"/>
+    <mergeCell ref="A339:D339"/>
+    <mergeCell ref="A338:D338"/>
+    <mergeCell ref="A344:D344"/>
+    <mergeCell ref="A290:D290"/>
+    <mergeCell ref="A292:D292"/>
+    <mergeCell ref="A291:D291"/>
+    <mergeCell ref="A295:D295"/>
+    <mergeCell ref="A296:D296"/>
+    <mergeCell ref="A300:D300"/>
+    <mergeCell ref="A301:D301"/>
+    <mergeCell ref="A345:D345"/>
+    <mergeCell ref="A346:D346"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A159:D159"/>
+    <mergeCell ref="A201:D201"/>
+    <mergeCell ref="A205:D205"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A187:D187"/>
+    <mergeCell ref="A188:D188"/>
+    <mergeCell ref="A192:D192"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A388:D388"/>
+    <mergeCell ref="A194:D194"/>
+    <mergeCell ref="A195:D195"/>
+    <mergeCell ref="A215:D215"/>
+    <mergeCell ref="A219:D219"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A319:D319"/>
+    <mergeCell ref="A272:D272"/>
+    <mergeCell ref="A273:D273"/>
+    <mergeCell ref="A274:D274"/>
+    <mergeCell ref="A279:D279"/>
+    <mergeCell ref="A347:D347"/>
+    <mergeCell ref="A353:D353"/>
+    <mergeCell ref="A325:D325"/>
+    <mergeCell ref="A326:D326"/>
+    <mergeCell ref="A280:D280"/>
+    <mergeCell ref="A282:D282"/>
+    <mergeCell ref="A283:D283"/>
+    <mergeCell ref="A309:D309"/>
+    <mergeCell ref="A310:D310"/>
+    <mergeCell ref="A366:D366"/>
+    <mergeCell ref="A316:D316"/>
+    <mergeCell ref="A355:D355"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A107:D107"/>
     <mergeCell ref="A391:D391"/>
     <mergeCell ref="A262:D262"/>
     <mergeCell ref="A235:D235"/>
@@ -27067,179 +27216,30 @@
     <mergeCell ref="A224:D224"/>
     <mergeCell ref="A226:D226"/>
     <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A323:D323"/>
+    <mergeCell ref="A358:D358"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A268:D268"/>
+    <mergeCell ref="A269:D269"/>
+    <mergeCell ref="A271:D271"/>
+    <mergeCell ref="A206:D206"/>
+    <mergeCell ref="A210:D210"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="A288:D288"/>
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A212:D212"/>
+    <mergeCell ref="A213:D213"/>
+    <mergeCell ref="A214:D214"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
     <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A165:D165"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A160:D160"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A388:D388"/>
-    <mergeCell ref="A194:D194"/>
-    <mergeCell ref="A195:D195"/>
-    <mergeCell ref="A215:D215"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A319:D319"/>
-    <mergeCell ref="A272:D272"/>
-    <mergeCell ref="A273:D273"/>
-    <mergeCell ref="A274:D274"/>
-    <mergeCell ref="A279:D279"/>
-    <mergeCell ref="A347:D347"/>
-    <mergeCell ref="A353:D353"/>
-    <mergeCell ref="A325:D325"/>
-    <mergeCell ref="A326:D326"/>
-    <mergeCell ref="A280:D280"/>
-    <mergeCell ref="A282:D282"/>
-    <mergeCell ref="A283:D283"/>
-    <mergeCell ref="A309:D309"/>
-    <mergeCell ref="A310:D310"/>
-    <mergeCell ref="A366:D366"/>
-    <mergeCell ref="A316:D316"/>
-    <mergeCell ref="A355:D355"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A159:D159"/>
-    <mergeCell ref="A201:D201"/>
-    <mergeCell ref="A205:D205"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="A181:D181"/>
-    <mergeCell ref="A187:D187"/>
-    <mergeCell ref="A188:D188"/>
-    <mergeCell ref="A192:D192"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A356:D356"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A240:D240"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="A244:D244"/>
-    <mergeCell ref="A246:D246"/>
-    <mergeCell ref="A247:D247"/>
-    <mergeCell ref="A251:D251"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A324:D324"/>
-    <mergeCell ref="A329:D329"/>
-    <mergeCell ref="A339:D339"/>
-    <mergeCell ref="A338:D338"/>
-    <mergeCell ref="A344:D344"/>
-    <mergeCell ref="A290:D290"/>
-    <mergeCell ref="A292:D292"/>
-    <mergeCell ref="A291:D291"/>
-    <mergeCell ref="A295:D295"/>
-    <mergeCell ref="A296:D296"/>
-    <mergeCell ref="A300:D300"/>
-    <mergeCell ref="A301:D301"/>
-    <mergeCell ref="A345:D345"/>
-    <mergeCell ref="A346:D346"/>
-    <mergeCell ref="A387:D387"/>
-    <mergeCell ref="A409:D409"/>
-    <mergeCell ref="A410:D410"/>
-    <mergeCell ref="A415:D415"/>
-    <mergeCell ref="A416:D416"/>
-    <mergeCell ref="A423:D423"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A174:D174"/>
-    <mergeCell ref="A418:D418"/>
-    <mergeCell ref="A354:D354"/>
-    <mergeCell ref="A322:D322"/>
-    <mergeCell ref="A328:D328"/>
-    <mergeCell ref="A303:D303"/>
-    <mergeCell ref="A304:D304"/>
-    <mergeCell ref="A306:D306"/>
-    <mergeCell ref="A305:D305"/>
-    <mergeCell ref="A307:D307"/>
-    <mergeCell ref="A308:D308"/>
-    <mergeCell ref="A357:D357"/>
-    <mergeCell ref="A365:D365"/>
-    <mergeCell ref="A403:D403"/>
-    <mergeCell ref="A404:D404"/>
-    <mergeCell ref="A369:D369"/>
-    <mergeCell ref="A394:D394"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A417:D417"/>
-    <mergeCell ref="A389:D389"/>
-    <mergeCell ref="A286:D286"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A320:D320"/>
-    <mergeCell ref="A321:D321"/>
-    <mergeCell ref="A200:D200"/>
-    <mergeCell ref="A232:D232"/>
-    <mergeCell ref="A233:D233"/>
-    <mergeCell ref="A236:D236"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A259:D259"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A379:D379"/>
-    <mergeCell ref="A380:D380"/>
-    <mergeCell ref="A386:D386"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="A397:D397"/>
-    <mergeCell ref="A359:D359"/>
-    <mergeCell ref="A390:D390"/>
-    <mergeCell ref="A392:D392"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A203:D203"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A370:D370"/>
-    <mergeCell ref="A373:D373"/>
-    <mergeCell ref="A374:D374"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A261:D261"/>
-    <mergeCell ref="A393:D393"/>
-    <mergeCell ref="A396:D396"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <conditionalFormatting sqref="M32:T32 M56:T77 M79:T104 M201:T232 M234:T259 M261:T286 M288:T320 M390:T1048576 M48:T48 M53:T54 M14:T14 M29:T29 M322:T355 M143:T165 M357:T388 M167:T199 M16:T23 Q15:T15 M34:T45 M106:T141">
     <cfRule type="cellIs" dxfId="175" priority="269" operator="equal">
@@ -27655,8 +27655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87786A15-F039-4732-8224-D8AE4342938B}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29685,7 +29685,9 @@
       <c r="A50" s="18" t="s">
         <v>383</v>
       </c>
-      <c r="B50" s="32"/>
+      <c r="B50" s="32" t="s">
+        <v>196</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>154</v>
       </c>
@@ -31859,7 +31861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2944F1E-C26E-4F90-A95D-D6E10706BE4A}">
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improved serving count calculation
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lg\repos\leonardguy\dunedin-zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1BF9C-CED5-4946-B15F-2880CB4D0983}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E613B9C7-C973-440E-B40A-6F3F839F850A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" activeTab="3" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11520" xr2:uid="{222B344E-0651-4EE9-BCB8-5C41E8873491}"/>
   </bookViews>
   <sheets>
     <sheet name="numbers" sheetId="5" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="490">
   <si>
     <t>g</t>
   </si>
@@ -1637,6 +1637,87 @@
   </si>
   <si>
     <t>2x 50g packets left over from last year</t>
+  </si>
+  <si>
+    <t>rice porridge</t>
+  </si>
+  <si>
+    <t>fruit salad</t>
+  </si>
+  <si>
+    <t>gf bread</t>
+  </si>
+  <si>
+    <t>butter / milk / cheese</t>
+  </si>
+  <si>
+    <t>olivani / soymilk</t>
+  </si>
+  <si>
+    <t>salad</t>
+  </si>
+  <si>
+    <t>Heidi = only eating porridge (normal), salad, and rice – weekend only</t>
+  </si>
+  <si>
+    <t>Diane = no sensitivities – weekend only</t>
+  </si>
+  <si>
+    <t>Neil = no sensitivities – weekend only</t>
+  </si>
+  <si>
+    <t>Leonard = no sensitivities</t>
+  </si>
+  <si>
+    <t>Caroline = no sensitivities</t>
+  </si>
+  <si>
+    <t>Kathy = no sensitivities</t>
+  </si>
+  <si>
+    <t>Damien = no sensitivities</t>
+  </si>
+  <si>
+    <t>Scott = no sensitivities (can’t eat pumpkin)</t>
+  </si>
+  <si>
+    <t>Claire = dairy free</t>
+  </si>
+  <si>
+    <t>Glenn = dairy free</t>
+  </si>
+  <si>
+    <t>Frances = dairy free</t>
+  </si>
+  <si>
+    <t>Gabrielle = gluten free</t>
+  </si>
+  <si>
+    <t>Lisa = gluten free</t>
+  </si>
+  <si>
+    <t>Malgoshia = no corn, gluten and dairy free</t>
+  </si>
+  <si>
+    <t>Jim = gluten and dairy free. Only person eating safe meal</t>
+  </si>
+  <si>
+    <t>weekend total eaters</t>
+  </si>
+  <si>
+    <t>weekday total eaters</t>
+  </si>
+  <si>
+    <t>weekend meal involved</t>
+  </si>
+  <si>
+    <t>weekday meals involved</t>
+  </si>
+  <si>
+    <t>jim having safe meal for dinner and lunch?</t>
+  </si>
+  <si>
+    <t>weekend only people leave after Sunday dinner?</t>
   </si>
 </sst>
 </file>
@@ -2227,7 +2308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2465,23 +2546,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="12" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4681,10 +4763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25A565D-02FB-480E-870E-F643EB26C74A}">
-  <dimension ref="A2:L9"/>
+  <dimension ref="A2:Z41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4698,12 +4780,26 @@
     <col min="8" max="8" width="7.7109375" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.28515625" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="28"/>
-    <col min="11" max="11" width="5.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="28"/>
+    <col min="13" max="13" width="56.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" style="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="28"/>
+    <col min="24" max="24" width="5.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="75" t="s">
         <v>329</v>
       </c>
@@ -4729,7 +4825,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>336</v>
       </c>
@@ -4765,7 +4861,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>337</v>
       </c>
@@ -4801,7 +4897,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>338</v>
       </c>
@@ -4835,7 +4931,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>339</v>
       </c>
@@ -4869,7 +4965,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>340</v>
       </c>
@@ -4903,7 +4999,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>341</v>
       </c>
@@ -4937,7 +5033,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="80" t="s">
         <v>314</v>
       </c>
@@ -4958,6 +5054,830 @@
       </c>
       <c r="H9" s="82" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N12" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="O12" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="P12" s="28" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="R12" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="S12" s="74" t="s">
+        <v>466</v>
+      </c>
+      <c r="T12" s="35" t="s">
+        <v>467</v>
+      </c>
+      <c r="U12" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="V12" s="74" t="s">
+        <v>338</v>
+      </c>
+      <c r="W12" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="X12" s="28" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y12" s="74" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z12" s="35" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="M13" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="N13" s="28">
+        <v>1</v>
+      </c>
+      <c r="O13" s="35"/>
+      <c r="P13" s="28">
+        <v>1</v>
+      </c>
+      <c r="R13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="28">
+        <v>1</v>
+      </c>
+      <c r="V13" s="74"/>
+      <c r="W13" s="35"/>
+      <c r="X13" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="35"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="M14" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="N14" s="28">
+        <v>1</v>
+      </c>
+      <c r="O14" s="35"/>
+      <c r="P14" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>1</v>
+      </c>
+      <c r="R14" s="35"/>
+      <c r="S14" s="28">
+        <v>1</v>
+      </c>
+      <c r="T14" s="35"/>
+      <c r="U14" s="28">
+        <v>1</v>
+      </c>
+      <c r="V14" s="74">
+        <v>1</v>
+      </c>
+      <c r="W14" s="35"/>
+      <c r="X14" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="35"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="M15" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="N15" s="28">
+        <v>1</v>
+      </c>
+      <c r="O15" s="35"/>
+      <c r="P15" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>1</v>
+      </c>
+      <c r="R15" s="35"/>
+      <c r="S15" s="28">
+        <v>1</v>
+      </c>
+      <c r="T15" s="35"/>
+      <c r="U15" s="28">
+        <v>1</v>
+      </c>
+      <c r="V15" s="74">
+        <v>1</v>
+      </c>
+      <c r="W15" s="35"/>
+      <c r="X15" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="35"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="M16" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="N16" s="28">
+        <v>1</v>
+      </c>
+      <c r="O16" s="35"/>
+      <c r="P16" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>1</v>
+      </c>
+      <c r="R16" s="35"/>
+      <c r="S16" s="28">
+        <v>1</v>
+      </c>
+      <c r="T16" s="35"/>
+      <c r="U16" s="28">
+        <v>1</v>
+      </c>
+      <c r="V16" s="74">
+        <v>1</v>
+      </c>
+      <c r="W16" s="35"/>
+      <c r="X16" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="35"/>
+    </row>
+    <row r="17" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M17" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="N17" s="28">
+        <v>1</v>
+      </c>
+      <c r="O17" s="35"/>
+      <c r="P17" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>1</v>
+      </c>
+      <c r="R17" s="35"/>
+      <c r="S17" s="28">
+        <v>1</v>
+      </c>
+      <c r="T17" s="35"/>
+      <c r="U17" s="28">
+        <v>1</v>
+      </c>
+      <c r="V17" s="74">
+        <v>1</v>
+      </c>
+      <c r="W17" s="35"/>
+      <c r="X17" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="35"/>
+    </row>
+    <row r="18" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M18" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="N18" s="28">
+        <v>1</v>
+      </c>
+      <c r="O18" s="35"/>
+      <c r="P18" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>1</v>
+      </c>
+      <c r="R18" s="35"/>
+      <c r="S18" s="28">
+        <v>1</v>
+      </c>
+      <c r="T18" s="35"/>
+      <c r="U18" s="28">
+        <v>1</v>
+      </c>
+      <c r="V18" s="74">
+        <v>1</v>
+      </c>
+      <c r="W18" s="35"/>
+      <c r="X18" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="35"/>
+    </row>
+    <row r="19" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M19" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="N19" s="28">
+        <v>1</v>
+      </c>
+      <c r="O19" s="35"/>
+      <c r="P19" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>1</v>
+      </c>
+      <c r="R19" s="35"/>
+      <c r="S19" s="28">
+        <v>1</v>
+      </c>
+      <c r="T19" s="35"/>
+      <c r="U19" s="28">
+        <v>1</v>
+      </c>
+      <c r="V19" s="74">
+        <v>1</v>
+      </c>
+      <c r="W19" s="35"/>
+      <c r="X19" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="35"/>
+    </row>
+    <row r="20" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M20" s="28" t="s">
+        <v>476</v>
+      </c>
+      <c r="N20" s="28">
+        <v>1</v>
+      </c>
+      <c r="O20" s="35"/>
+      <c r="P20" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="28">
+        <v>1</v>
+      </c>
+      <c r="R20" s="35"/>
+      <c r="S20" s="28">
+        <v>1</v>
+      </c>
+      <c r="T20" s="35"/>
+      <c r="U20" s="28">
+        <v>1</v>
+      </c>
+      <c r="V20" s="74">
+        <v>1</v>
+      </c>
+      <c r="W20" s="35"/>
+      <c r="X20" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="35"/>
+    </row>
+    <row r="21" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M21" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="N21" s="28">
+        <v>1</v>
+      </c>
+      <c r="O21" s="35"/>
+      <c r="P21" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="28">
+        <v>1</v>
+      </c>
+      <c r="R21" s="35"/>
+      <c r="T21" s="35">
+        <v>1</v>
+      </c>
+      <c r="U21" s="28">
+        <v>1</v>
+      </c>
+      <c r="V21" s="74">
+        <v>1</v>
+      </c>
+      <c r="W21" s="35"/>
+      <c r="X21" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="35"/>
+    </row>
+    <row r="22" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M22" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="N22" s="28">
+        <v>1</v>
+      </c>
+      <c r="O22" s="35"/>
+      <c r="P22" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="28">
+        <v>1</v>
+      </c>
+      <c r="R22" s="35"/>
+      <c r="T22" s="35">
+        <v>1</v>
+      </c>
+      <c r="U22" s="28">
+        <v>1</v>
+      </c>
+      <c r="V22" s="74">
+        <v>1</v>
+      </c>
+      <c r="W22" s="35"/>
+      <c r="X22" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="35"/>
+    </row>
+    <row r="23" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M23" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="N23" s="28">
+        <v>1</v>
+      </c>
+      <c r="O23" s="35"/>
+      <c r="P23" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="28">
+        <v>1</v>
+      </c>
+      <c r="R23" s="35"/>
+      <c r="T23" s="35">
+        <v>1</v>
+      </c>
+      <c r="U23" s="28">
+        <v>1</v>
+      </c>
+      <c r="V23" s="74">
+        <v>1</v>
+      </c>
+      <c r="W23" s="35"/>
+      <c r="X23" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="35"/>
+    </row>
+    <row r="24" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M24" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="O24" s="35">
+        <v>1</v>
+      </c>
+      <c r="P24" s="28">
+        <v>1</v>
+      </c>
+      <c r="R24" s="35">
+        <v>1</v>
+      </c>
+      <c r="S24" s="28">
+        <v>1</v>
+      </c>
+      <c r="T24" s="35"/>
+      <c r="U24" s="28">
+        <v>1</v>
+      </c>
+      <c r="V24" s="74">
+        <v>1</v>
+      </c>
+      <c r="W24" s="35"/>
+      <c r="X24" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="35"/>
+    </row>
+    <row r="25" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M25" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="O25" s="35">
+        <v>1</v>
+      </c>
+      <c r="P25" s="28">
+        <v>1</v>
+      </c>
+      <c r="R25" s="35">
+        <v>1</v>
+      </c>
+      <c r="S25" s="28">
+        <v>1</v>
+      </c>
+      <c r="T25" s="35"/>
+      <c r="U25" s="28">
+        <v>1</v>
+      </c>
+      <c r="V25" s="74">
+        <v>1</v>
+      </c>
+      <c r="W25" s="35"/>
+      <c r="X25" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="35"/>
+    </row>
+    <row r="26" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M26" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="O26" s="35">
+        <v>1</v>
+      </c>
+      <c r="P26" s="28">
+        <v>1</v>
+      </c>
+      <c r="R26" s="35">
+        <v>1</v>
+      </c>
+      <c r="T26" s="35">
+        <v>1</v>
+      </c>
+      <c r="U26" s="28">
+        <v>1</v>
+      </c>
+      <c r="V26" s="74">
+        <v>1</v>
+      </c>
+      <c r="W26" s="35"/>
+      <c r="X26" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="35"/>
+    </row>
+    <row r="27" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M27" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="O27" s="35">
+        <v>1</v>
+      </c>
+      <c r="P27" s="28">
+        <v>1</v>
+      </c>
+      <c r="R27" s="35">
+        <v>1</v>
+      </c>
+      <c r="T27" s="35">
+        <v>1</v>
+      </c>
+      <c r="U27" s="28">
+        <v>1</v>
+      </c>
+      <c r="V27" s="74"/>
+      <c r="W27" s="35">
+        <v>1</v>
+      </c>
+      <c r="X27" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="74"/>
+      <c r="Z27" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="O28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="35"/>
+      <c r="Y28" s="74"/>
+      <c r="Z28" s="35"/>
+    </row>
+    <row r="29" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M29" s="74" t="s">
+        <v>484</v>
+      </c>
+      <c r="N29" s="28">
+        <f>SUM(N13:N27)</f>
+        <v>11</v>
+      </c>
+      <c r="O29" s="35">
+        <f t="shared" ref="O29:Z29" si="1">SUM(O13:O27)</f>
+        <v>4</v>
+      </c>
+      <c r="P29" s="28">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Q29" s="28">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="R29" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S29" s="28">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="T29" s="35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="U29" s="28">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="V29" s="74">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="W29" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X29" s="28">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Y29" s="74">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Z29" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M30" s="74" t="s">
+        <v>485</v>
+      </c>
+      <c r="N30" s="28">
+        <f>N29-N13-N14-N15</f>
+        <v>8</v>
+      </c>
+      <c r="O30" s="35">
+        <f t="shared" ref="O30:Z30" si="2">O29-O13-O14-O15</f>
+        <v>4</v>
+      </c>
+      <c r="P30" s="28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Q30" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="R30" s="35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="S30" s="28">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="T30" s="35">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="U30" s="28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="V30" s="74">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="W30" s="35">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="X30" s="28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Y30" s="74">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Z30" s="35">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="O31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="35"/>
+      <c r="Y31" s="74"/>
+      <c r="Z31" s="35"/>
+    </row>
+    <row r="32" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M32" s="74" t="s">
+        <v>486</v>
+      </c>
+      <c r="N32" s="28">
+        <v>2</v>
+      </c>
+      <c r="O32" s="35">
+        <v>2</v>
+      </c>
+      <c r="P32" s="74">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="74">
+        <v>4</v>
+      </c>
+      <c r="R32" s="35">
+        <v>4</v>
+      </c>
+      <c r="S32" s="28">
+        <v>4</v>
+      </c>
+      <c r="T32" s="35">
+        <v>9</v>
+      </c>
+      <c r="U32" s="28">
+        <v>2</v>
+      </c>
+      <c r="V32" s="74">
+        <v>2</v>
+      </c>
+      <c r="W32" s="35">
+        <v>2</v>
+      </c>
+      <c r="X32" s="28">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="74">
+        <v>2</v>
+      </c>
+      <c r="Z32" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M33" s="74" t="s">
+        <v>487</v>
+      </c>
+      <c r="N33" s="28">
+        <v>5</v>
+      </c>
+      <c r="O33" s="35">
+        <v>5</v>
+      </c>
+      <c r="P33" s="28">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="28">
+        <v>9</v>
+      </c>
+      <c r="R33" s="35">
+        <v>9</v>
+      </c>
+      <c r="S33" s="28">
+        <v>4</v>
+      </c>
+      <c r="T33" s="35">
+        <v>9</v>
+      </c>
+      <c r="U33" s="28">
+        <v>4</v>
+      </c>
+      <c r="V33" s="74">
+        <v>4</v>
+      </c>
+      <c r="W33" s="35">
+        <v>4</v>
+      </c>
+      <c r="X33" s="28">
+        <v>4</v>
+      </c>
+      <c r="Y33" s="74">
+        <v>4</v>
+      </c>
+      <c r="Z33" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="O34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="35"/>
+      <c r="Y34" s="74"/>
+      <c r="Z34" s="35"/>
+    </row>
+    <row r="35" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M35" s="74" t="s">
+        <v>327</v>
+      </c>
+      <c r="N35" s="28">
+        <f>N32*N29+N33*N30</f>
+        <v>62</v>
+      </c>
+      <c r="O35" s="35">
+        <f t="shared" ref="O35:Z35" si="3">O32*O29+O33*O30</f>
+        <v>28</v>
+      </c>
+      <c r="P35" s="28">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="Q35" s="28">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="R35" s="35">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="S35" s="28">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="T35" s="35">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="U35" s="28">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="V35" s="28">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="W35" s="35">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="X35" s="28">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="Y35" s="28">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="Z35" s="35">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M40" s="122" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="41" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M41" s="122" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -5006,12 +5926,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="102" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="116" t="s">
         <v>431</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
       <c r="E1" s="40" t="s">
         <v>413</v>
       </c>
@@ -5033,12 +5953,12 @@
       <c r="Z1" s="46"/>
     </row>
     <row r="2" spans="1:30" s="102" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="116" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
       <c r="E2" s="100" t="s">
         <v>53</v>
       </c>
@@ -5114,13 +6034,13 @@
       </c>
     </row>
     <row r="3" spans="1:30" s="102" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="str">
+      <c r="A3" s="117" t="str">
         <f>_xlfn.CONCAT(F3," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
       <c r="E3" s="100" t="s">
         <v>348</v>
       </c>
@@ -5750,12 +6670,12 @@
       <c r="Z13" s="46"/>
     </row>
     <row r="14" spans="1:30" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="116" t="s">
         <v>429</v>
       </c>
-      <c r="B14" s="117"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
       <c r="E14" s="40" t="s">
         <v>303</v>
       </c>
@@ -5777,12 +6697,12 @@
       <c r="Z14" s="46"/>
     </row>
     <row r="15" spans="1:30" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="116" t="s">
         <v>430</v>
       </c>
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
       <c r="E15" s="63" t="s">
         <v>53</v>
       </c>
@@ -5858,13 +6778,13 @@
       </c>
     </row>
     <row r="16" spans="1:30" s="64" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="118" t="str">
+      <c r="A16" s="117" t="str">
         <f>_xlfn.CONCAT(F16," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
       <c r="E16" s="63" t="s">
         <v>348</v>
       </c>
@@ -6777,12 +7697,12 @@
       <c r="Z31" s="46"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="116"/>
+      <c r="D32" s="116"/>
       <c r="E32" s="40" t="s">
         <v>184</v>
       </c>
@@ -6790,12 +7710,12 @@
       <c r="G32" s="100"/>
     </row>
     <row r="33" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="116" t="s">
         <v>384</v>
       </c>
-      <c r="B33" s="117"/>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
       <c r="E33" s="39" t="s">
         <v>53</v>
       </c>
@@ -6871,13 +7791,13 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="118" t="str">
+      <c r="A34" s="117" t="str">
         <f>_xlfn.CONCAT(F34," servings")</f>
         <v>4 servings</v>
       </c>
-      <c r="B34" s="118"/>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
       <c r="E34" s="39" t="s">
         <v>348</v>
       </c>
@@ -8116,12 +9036,12 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="117" t="s">
+      <c r="A54" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="117"/>
-      <c r="C54" s="117"/>
-      <c r="D54" s="117"/>
+      <c r="B54" s="116"/>
+      <c r="C54" s="116"/>
+      <c r="D54" s="116"/>
       <c r="E54" s="39" t="s">
         <v>125</v>
       </c>
@@ -8131,12 +9051,12 @@
       <c r="G54" s="100"/>
     </row>
     <row r="55" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="121" t="s">
+      <c r="A55" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="121"/>
-      <c r="C55" s="121"/>
-      <c r="D55" s="121"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
       <c r="E55" s="39" t="s">
         <v>53</v>
       </c>
@@ -8213,13 +9133,13 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="118" t="str">
+      <c r="A56" s="117" t="str">
         <f>_xlfn.CONCAT(F56," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B56" s="118"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="118"/>
+      <c r="B56" s="117"/>
+      <c r="C56" s="117"/>
+      <c r="D56" s="117"/>
       <c r="E56" s="63" t="s">
         <v>348</v>
       </c>
@@ -9292,12 +10212,12 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="117" t="s">
+      <c r="A77" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B77" s="117"/>
-      <c r="C77" s="117"/>
-      <c r="D77" s="117"/>
+      <c r="B77" s="116"/>
+      <c r="C77" s="116"/>
+      <c r="D77" s="116"/>
       <c r="E77" s="57" t="s">
         <v>126</v>
       </c>
@@ -9307,12 +10227,12 @@
       <c r="G77" s="100"/>
     </row>
     <row r="78" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A78" s="117" t="s">
+      <c r="A78" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="117"/>
-      <c r="C78" s="117"/>
-      <c r="D78" s="117"/>
+      <c r="B78" s="116"/>
+      <c r="C78" s="116"/>
+      <c r="D78" s="116"/>
       <c r="E78" s="39" t="s">
         <v>53</v>
       </c>
@@ -9387,13 +10307,13 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="118" t="str">
+      <c r="A79" s="117" t="str">
         <f>_xlfn.CONCAT(F79," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B79" s="118"/>
-      <c r="C79" s="118"/>
-      <c r="D79" s="118"/>
+      <c r="B79" s="117"/>
+      <c r="C79" s="117"/>
+      <c r="D79" s="117"/>
       <c r="E79" s="63" t="s">
         <v>348</v>
       </c>
@@ -10703,12 +11623,12 @@
       <c r="P103" s="41"/>
     </row>
     <row r="104" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="117" t="s">
+      <c r="A104" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="B104" s="117"/>
-      <c r="C104" s="117"/>
-      <c r="D104" s="117"/>
+      <c r="B104" s="116"/>
+      <c r="C104" s="116"/>
+      <c r="D104" s="116"/>
       <c r="E104" s="40" t="s">
         <v>132</v>
       </c>
@@ -10719,12 +11639,12 @@
       <c r="I104" s="44"/>
     </row>
     <row r="105" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A105" s="117" t="s">
+      <c r="A105" s="116" t="s">
         <v>263</v>
       </c>
-      <c r="B105" s="117"/>
-      <c r="C105" s="117"/>
-      <c r="D105" s="117"/>
+      <c r="B105" s="116"/>
+      <c r="C105" s="116"/>
+      <c r="D105" s="116"/>
       <c r="E105" s="39" t="s">
         <v>53</v>
       </c>
@@ -10801,13 +11721,13 @@
       </c>
     </row>
     <row r="106" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="118" t="str">
+      <c r="A106" s="117" t="str">
         <f>_xlfn.CONCAT(F106," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B106" s="118"/>
-      <c r="C106" s="118"/>
-      <c r="D106" s="118"/>
+      <c r="B106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
       <c r="E106" s="63" t="s">
         <v>348</v>
       </c>
@@ -12365,12 +13285,12 @@
       </c>
     </row>
     <row r="141" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="117" t="s">
+      <c r="A141" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B141" s="117"/>
-      <c r="C141" s="117"/>
-      <c r="D141" s="117"/>
+      <c r="B141" s="116"/>
+      <c r="C141" s="116"/>
+      <c r="D141" s="116"/>
       <c r="E141" s="40" t="s">
         <v>127</v>
       </c>
@@ -12381,12 +13301,12 @@
       <c r="H141" s="44"/>
     </row>
     <row r="142" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A142" s="117" t="s">
+      <c r="A142" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="B142" s="117"/>
-      <c r="C142" s="117"/>
-      <c r="D142" s="117"/>
+      <c r="B142" s="116"/>
+      <c r="C142" s="116"/>
+      <c r="D142" s="116"/>
       <c r="E142" s="39" t="s">
         <v>53</v>
       </c>
@@ -12463,13 +13383,13 @@
       </c>
     </row>
     <row r="143" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="118" t="str">
+      <c r="A143" s="117" t="str">
         <f>_xlfn.CONCAT(F143," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B143" s="118"/>
-      <c r="C143" s="118"/>
-      <c r="D143" s="118"/>
+      <c r="B143" s="117"/>
+      <c r="C143" s="117"/>
+      <c r="D143" s="117"/>
       <c r="E143" s="63" t="s">
         <v>348</v>
       </c>
@@ -13649,12 +14569,12 @@
       </c>
     </row>
     <row r="165" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="117" t="s">
+      <c r="A165" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="B165" s="117"/>
-      <c r="C165" s="117"/>
-      <c r="D165" s="117"/>
+      <c r="B165" s="116"/>
+      <c r="C165" s="116"/>
+      <c r="D165" s="116"/>
       <c r="E165" s="40" t="s">
         <v>134</v>
       </c>
@@ -13664,12 +14584,12 @@
       <c r="G165" s="100"/>
     </row>
     <row r="166" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A166" s="117" t="s">
+      <c r="A166" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="B166" s="117"/>
-      <c r="C166" s="117"/>
-      <c r="D166" s="117"/>
+      <c r="B166" s="116"/>
+      <c r="C166" s="116"/>
+      <c r="D166" s="116"/>
       <c r="E166" s="39" t="s">
         <v>53</v>
       </c>
@@ -13745,13 +14665,13 @@
       </c>
     </row>
     <row r="167" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="118" t="str">
+      <c r="A167" s="117" t="str">
         <f>_xlfn.CONCAT(F167," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B167" s="118"/>
-      <c r="C167" s="118"/>
-      <c r="D167" s="118"/>
+      <c r="B167" s="117"/>
+      <c r="C167" s="117"/>
+      <c r="D167" s="117"/>
       <c r="E167" s="63" t="s">
         <v>348</v>
       </c>
@@ -15637,12 +16557,12 @@
       </c>
     </row>
     <row r="199" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="117" t="s">
+      <c r="A199" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="B199" s="117"/>
-      <c r="C199" s="117"/>
-      <c r="D199" s="117"/>
+      <c r="B199" s="116"/>
+      <c r="C199" s="116"/>
+      <c r="D199" s="116"/>
       <c r="E199" s="40" t="s">
         <v>129</v>
       </c>
@@ -15653,12 +16573,12 @@
       <c r="H199" s="44"/>
     </row>
     <row r="200" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A200" s="117" t="s">
+      <c r="A200" s="116" t="s">
         <v>249</v>
       </c>
-      <c r="B200" s="117"/>
-      <c r="C200" s="117"/>
-      <c r="D200" s="117"/>
+      <c r="B200" s="116"/>
+      <c r="C200" s="116"/>
+      <c r="D200" s="116"/>
       <c r="E200" s="39" t="s">
         <v>53</v>
       </c>
@@ -15735,13 +16655,13 @@
       </c>
     </row>
     <row r="201" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="118" t="str">
+      <c r="A201" s="117" t="str">
         <f>_xlfn.CONCAT(F201," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B201" s="118"/>
-      <c r="C201" s="118"/>
-      <c r="D201" s="118"/>
+      <c r="B201" s="117"/>
+      <c r="C201" s="117"/>
+      <c r="D201" s="117"/>
       <c r="E201" s="63" t="s">
         <v>348</v>
       </c>
@@ -15929,10 +16849,10 @@
       </c>
     </row>
     <row r="205" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="116"/>
-      <c r="B205" s="116"/>
-      <c r="C205" s="116"/>
-      <c r="D205" s="116"/>
+      <c r="A205" s="119"/>
+      <c r="B205" s="119"/>
+      <c r="C205" s="119"/>
+      <c r="D205" s="119"/>
       <c r="E205" s="63" t="s">
         <v>352</v>
       </c>
@@ -16236,10 +17156,10 @@
       </c>
     </row>
     <row r="210" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="116"/>
-      <c r="B210" s="116"/>
-      <c r="C210" s="116"/>
-      <c r="D210" s="116"/>
+      <c r="A210" s="119"/>
+      <c r="B210" s="119"/>
+      <c r="C210" s="119"/>
+      <c r="D210" s="119"/>
       <c r="E210" s="39"/>
       <c r="F210" s="39"/>
       <c r="G210" s="44"/>
@@ -16300,10 +17220,10 @@
       <c r="AD211" s="71"/>
     </row>
     <row r="212" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="116"/>
-      <c r="B212" s="116"/>
-      <c r="C212" s="116"/>
-      <c r="D212" s="116"/>
+      <c r="A212" s="119"/>
+      <c r="B212" s="119"/>
+      <c r="C212" s="119"/>
+      <c r="D212" s="119"/>
       <c r="E212" s="39"/>
       <c r="F212" s="39"/>
       <c r="G212" s="44"/>
@@ -16364,10 +17284,10 @@
       <c r="AD213" s="71"/>
     </row>
     <row r="214" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="116"/>
-      <c r="B214" s="116"/>
-      <c r="C214" s="116"/>
-      <c r="D214" s="116"/>
+      <c r="A214" s="119"/>
+      <c r="B214" s="119"/>
+      <c r="C214" s="119"/>
+      <c r="D214" s="119"/>
       <c r="E214" s="39"/>
       <c r="F214" s="39"/>
       <c r="G214" s="44"/>
@@ -16706,10 +17626,10 @@
       </c>
     </row>
     <row r="219" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="116"/>
-      <c r="B219" s="116"/>
-      <c r="C219" s="116"/>
-      <c r="D219" s="116"/>
+      <c r="A219" s="119"/>
+      <c r="B219" s="119"/>
+      <c r="C219" s="119"/>
+      <c r="D219" s="119"/>
       <c r="E219" s="39"/>
       <c r="F219" s="39"/>
       <c r="G219" s="44"/>
@@ -17228,12 +18148,12 @@
       </c>
     </row>
     <row r="232" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A232" s="117" t="s">
+      <c r="A232" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="B232" s="117"/>
-      <c r="C232" s="117"/>
-      <c r="D232" s="117"/>
+      <c r="B232" s="116"/>
+      <c r="C232" s="116"/>
+      <c r="D232" s="116"/>
       <c r="E232" s="40" t="s">
         <v>130</v>
       </c>
@@ -17244,12 +18164,12 @@
       <c r="H232" s="44"/>
     </row>
     <row r="233" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A233" s="117" t="s">
+      <c r="A233" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="B233" s="117"/>
-      <c r="C233" s="117"/>
-      <c r="D233" s="117"/>
+      <c r="B233" s="116"/>
+      <c r="C233" s="116"/>
+      <c r="D233" s="116"/>
       <c r="E233" s="39" t="s">
         <v>53</v>
       </c>
@@ -17326,13 +18246,13 @@
       </c>
     </row>
     <row r="234" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="118" t="str">
+      <c r="A234" s="117" t="str">
         <f>_xlfn.CONCAT(F234," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B234" s="118"/>
-      <c r="C234" s="118"/>
-      <c r="D234" s="118"/>
+      <c r="B234" s="117"/>
+      <c r="C234" s="117"/>
+      <c r="D234" s="117"/>
       <c r="E234" s="63" t="s">
         <v>348</v>
       </c>
@@ -18687,12 +19607,12 @@
       </c>
     </row>
     <row r="259" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A259" s="117" t="s">
+      <c r="A259" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B259" s="117"/>
-      <c r="C259" s="117"/>
-      <c r="D259" s="117"/>
+      <c r="B259" s="116"/>
+      <c r="C259" s="116"/>
+      <c r="D259" s="116"/>
       <c r="E259" s="40" t="s">
         <v>131</v>
       </c>
@@ -18703,12 +19623,12 @@
       <c r="H259" s="44"/>
     </row>
     <row r="260" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A260" s="117" t="s">
+      <c r="A260" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="B260" s="117"/>
-      <c r="C260" s="117"/>
-      <c r="D260" s="117"/>
+      <c r="B260" s="116"/>
+      <c r="C260" s="116"/>
+      <c r="D260" s="116"/>
       <c r="E260" s="39" t="s">
         <v>53</v>
       </c>
@@ -18785,13 +19705,13 @@
       </c>
     </row>
     <row r="261" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="118" t="str">
+      <c r="A261" s="117" t="str">
         <f>_xlfn.CONCAT(F261," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B261" s="118"/>
-      <c r="C261" s="118"/>
-      <c r="D261" s="118"/>
+      <c r="B261" s="117"/>
+      <c r="C261" s="117"/>
+      <c r="D261" s="117"/>
       <c r="E261" s="63" t="s">
         <v>348</v>
       </c>
@@ -19841,12 +20761,12 @@
       <c r="AD285" s="64"/>
     </row>
     <row r="286" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A286" s="117" t="s">
+      <c r="A286" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="B286" s="117"/>
-      <c r="C286" s="117"/>
-      <c r="D286" s="117"/>
+      <c r="B286" s="116"/>
+      <c r="C286" s="116"/>
+      <c r="D286" s="116"/>
       <c r="E286" s="39" t="s">
         <v>136</v>
       </c>
@@ -19855,12 +20775,12 @@
       <c r="H286" s="44"/>
     </row>
     <row r="287" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A287" s="117" t="s">
+      <c r="A287" s="116" t="s">
         <v>275</v>
       </c>
-      <c r="B287" s="117"/>
-      <c r="C287" s="117"/>
-      <c r="D287" s="117"/>
+      <c r="B287" s="116"/>
+      <c r="C287" s="116"/>
+      <c r="D287" s="116"/>
       <c r="E287" s="39" t="s">
         <v>53</v>
       </c>
@@ -19937,13 +20857,13 @@
       </c>
     </row>
     <row r="288" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="118" t="str">
+      <c r="A288" s="117" t="str">
         <f>_xlfn.CONCAT(F288," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B288" s="118"/>
-      <c r="C288" s="118"/>
-      <c r="D288" s="118"/>
+      <c r="B288" s="117"/>
+      <c r="C288" s="117"/>
+      <c r="D288" s="117"/>
       <c r="E288" s="63" t="s">
         <v>348</v>
       </c>
@@ -19984,12 +20904,12 @@
       <c r="Z289" s="46"/>
     </row>
     <row r="290" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A290" s="119" t="s">
+      <c r="A290" s="121" t="s">
         <v>276</v>
       </c>
-      <c r="B290" s="119"/>
-      <c r="C290" s="119"/>
-      <c r="D290" s="119"/>
+      <c r="B290" s="121"/>
+      <c r="C290" s="121"/>
+      <c r="D290" s="121"/>
       <c r="E290" s="64"/>
       <c r="F290" s="64"/>
       <c r="G290" s="64"/>
@@ -20718,12 +21638,12 @@
       <c r="AD305" s="71"/>
     </row>
     <row r="306" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A306" s="119" t="s">
+      <c r="A306" s="121" t="s">
         <v>281</v>
       </c>
-      <c r="B306" s="119"/>
-      <c r="C306" s="119"/>
-      <c r="D306" s="119"/>
+      <c r="B306" s="121"/>
+      <c r="C306" s="121"/>
+      <c r="D306" s="121"/>
       <c r="E306" s="40"/>
       <c r="F306" s="57"/>
       <c r="G306" s="57"/>
@@ -21340,12 +22260,12 @@
       <c r="H319" s="44"/>
     </row>
     <row r="320" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A320" s="117" t="s">
+      <c r="A320" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B320" s="117"/>
-      <c r="C320" s="117"/>
-      <c r="D320" s="117"/>
+      <c r="B320" s="116"/>
+      <c r="C320" s="116"/>
+      <c r="D320" s="116"/>
       <c r="E320" s="40" t="s">
         <v>133</v>
       </c>
@@ -21355,12 +22275,12 @@
       <c r="G320" s="100"/>
     </row>
     <row r="321" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A321" s="117" t="s">
+      <c r="A321" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B321" s="117"/>
-      <c r="C321" s="117"/>
-      <c r="D321" s="117"/>
+      <c r="B321" s="116"/>
+      <c r="C321" s="116"/>
+      <c r="D321" s="116"/>
       <c r="E321" s="39" t="s">
         <v>53</v>
       </c>
@@ -21436,13 +22356,13 @@
       </c>
     </row>
     <row r="322" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A322" s="118" t="str">
+      <c r="A322" s="117" t="str">
         <f>_xlfn.CONCAT(F322," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B322" s="118"/>
-      <c r="C322" s="118"/>
-      <c r="D322" s="118"/>
+      <c r="B322" s="117"/>
+      <c r="C322" s="117"/>
+      <c r="D322" s="117"/>
       <c r="E322" s="63" t="s">
         <v>348</v>
       </c>
@@ -23298,12 +24218,12 @@
       <c r="N354" s="41"/>
     </row>
     <row r="355" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A355" s="117" t="s">
+      <c r="A355" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="B355" s="117"/>
-      <c r="C355" s="117"/>
-      <c r="D355" s="117"/>
+      <c r="B355" s="116"/>
+      <c r="C355" s="116"/>
+      <c r="D355" s="116"/>
       <c r="E355" s="40" t="s">
         <v>128</v>
       </c>
@@ -23314,12 +24234,12 @@
       <c r="H355" s="44"/>
     </row>
     <row r="356" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A356" s="117" t="s">
+      <c r="A356" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="B356" s="117"/>
-      <c r="C356" s="117"/>
-      <c r="D356" s="117"/>
+      <c r="B356" s="116"/>
+      <c r="C356" s="116"/>
+      <c r="D356" s="116"/>
       <c r="E356" s="39" t="s">
         <v>53</v>
       </c>
@@ -23396,13 +24316,13 @@
       </c>
     </row>
     <row r="357" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A357" s="118" t="str">
+      <c r="A357" s="117" t="str">
         <f>_xlfn.CONCAT(F357," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B357" s="118"/>
-      <c r="C357" s="118"/>
-      <c r="D357" s="118"/>
+      <c r="B357" s="117"/>
+      <c r="C357" s="117"/>
+      <c r="D357" s="117"/>
       <c r="E357" s="63" t="s">
         <v>348</v>
       </c>
@@ -23970,10 +24890,10 @@
       </c>
     </row>
     <row r="365" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A365" s="116"/>
-      <c r="B365" s="116"/>
-      <c r="C365" s="116"/>
-      <c r="D365" s="116"/>
+      <c r="A365" s="119"/>
+      <c r="B365" s="119"/>
+      <c r="C365" s="119"/>
+      <c r="D365" s="119"/>
       <c r="E365" s="39"/>
       <c r="F365" s="39"/>
       <c r="G365" s="44"/>
@@ -24223,10 +25143,10 @@
       </c>
     </row>
     <row r="369" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A369" s="116"/>
-      <c r="B369" s="116"/>
-      <c r="C369" s="116"/>
-      <c r="D369" s="116"/>
+      <c r="A369" s="119"/>
+      <c r="B369" s="119"/>
+      <c r="C369" s="119"/>
+      <c r="D369" s="119"/>
       <c r="E369" s="39"/>
       <c r="F369" s="39"/>
       <c r="G369" s="44"/>
@@ -24467,10 +25387,10 @@
       </c>
     </row>
     <row r="373" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A373" s="116"/>
-      <c r="B373" s="116"/>
-      <c r="C373" s="116"/>
-      <c r="D373" s="116"/>
+      <c r="A373" s="119"/>
+      <c r="B373" s="119"/>
+      <c r="C373" s="119"/>
+      <c r="D373" s="119"/>
       <c r="E373" s="39"/>
       <c r="F373" s="39"/>
       <c r="G373" s="44"/>
@@ -24895,10 +25815,10 @@
       </c>
     </row>
     <row r="379" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A379" s="116"/>
-      <c r="B379" s="116"/>
-      <c r="C379" s="116"/>
-      <c r="D379" s="116"/>
+      <c r="A379" s="119"/>
+      <c r="B379" s="119"/>
+      <c r="C379" s="119"/>
+      <c r="D379" s="119"/>
       <c r="E379" s="39"/>
       <c r="F379" s="39"/>
       <c r="G379" s="44"/>
@@ -25319,10 +26239,10 @@
       </c>
     </row>
     <row r="386" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A386" s="116"/>
-      <c r="B386" s="116"/>
-      <c r="C386" s="116"/>
-      <c r="D386" s="116"/>
+      <c r="A386" s="119"/>
+      <c r="B386" s="119"/>
+      <c r="C386" s="119"/>
+      <c r="D386" s="119"/>
       <c r="E386" s="39"/>
       <c r="F386" s="39"/>
       <c r="G386" s="44"/>
@@ -25367,12 +26287,12 @@
       <c r="U387" s="39"/>
     </row>
     <row r="388" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A388" s="117" t="s">
+      <c r="A388" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="B388" s="117"/>
-      <c r="C388" s="117"/>
-      <c r="D388" s="117"/>
+      <c r="B388" s="116"/>
+      <c r="C388" s="116"/>
+      <c r="D388" s="116"/>
       <c r="E388" s="40" t="s">
         <v>135</v>
       </c>
@@ -25382,12 +26302,12 @@
       <c r="G388" s="100"/>
     </row>
     <row r="389" spans="1:30" ht="24" x14ac:dyDescent="0.2">
-      <c r="A389" s="117" t="s">
+      <c r="A389" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="B389" s="117"/>
-      <c r="C389" s="117"/>
-      <c r="D389" s="117"/>
+      <c r="B389" s="116"/>
+      <c r="C389" s="116"/>
+      <c r="D389" s="116"/>
       <c r="E389" s="39" t="s">
         <v>53</v>
       </c>
@@ -25463,13 +26383,13 @@
       </c>
     </row>
     <row r="390" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A390" s="118" t="str">
+      <c r="A390" s="117" t="str">
         <f>_xlfn.CONCAT(F390," servings")</f>
         <v>10 servings</v>
       </c>
-      <c r="B390" s="118"/>
-      <c r="C390" s="118"/>
-      <c r="D390" s="118"/>
+      <c r="B390" s="117"/>
+      <c r="C390" s="117"/>
+      <c r="D390" s="117"/>
       <c r="E390" s="63" t="s">
         <v>348</v>
       </c>
@@ -26893,12 +27813,12 @@
       <c r="Z416" s="41"/>
     </row>
     <row r="417" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A417" s="117" t="s">
+      <c r="A417" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="B417" s="117"/>
-      <c r="C417" s="117"/>
-      <c r="D417" s="117"/>
+      <c r="B417" s="116"/>
+      <c r="C417" s="116"/>
+      <c r="D417" s="116"/>
       <c r="M417" s="41"/>
       <c r="N417" s="41"/>
       <c r="O417" s="41"/>
@@ -26929,12 +27849,12 @@
       <c r="Z418" s="41"/>
     </row>
     <row r="423" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A423" s="117" t="s">
+      <c r="A423" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="B423" s="117"/>
-      <c r="C423" s="117"/>
-      <c r="D423" s="117"/>
+      <c r="B423" s="116"/>
+      <c r="C423" s="116"/>
+      <c r="D423" s="116"/>
       <c r="M423" s="41"/>
       <c r="N423" s="41"/>
       <c r="O423" s="41"/>
@@ -27020,17 +27940,191 @@
     </row>
   </sheetData>
   <mergeCells count="220">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A323:D323"/>
+    <mergeCell ref="A358:D358"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A268:D268"/>
+    <mergeCell ref="A269:D269"/>
+    <mergeCell ref="A271:D271"/>
+    <mergeCell ref="A206:D206"/>
+    <mergeCell ref="A210:D210"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="A288:D288"/>
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A212:D212"/>
+    <mergeCell ref="A213:D213"/>
+    <mergeCell ref="A214:D214"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A391:D391"/>
+    <mergeCell ref="A262:D262"/>
+    <mergeCell ref="A235:D235"/>
+    <mergeCell ref="A202:D202"/>
+    <mergeCell ref="A168:D168"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A317:D317"/>
+    <mergeCell ref="A318:D318"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A224:D224"/>
+    <mergeCell ref="A226:D226"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A388:D388"/>
+    <mergeCell ref="A194:D194"/>
+    <mergeCell ref="A195:D195"/>
+    <mergeCell ref="A215:D215"/>
+    <mergeCell ref="A219:D219"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A319:D319"/>
+    <mergeCell ref="A272:D272"/>
+    <mergeCell ref="A273:D273"/>
+    <mergeCell ref="A274:D274"/>
+    <mergeCell ref="A279:D279"/>
+    <mergeCell ref="A347:D347"/>
+    <mergeCell ref="A353:D353"/>
+    <mergeCell ref="A325:D325"/>
+    <mergeCell ref="A326:D326"/>
+    <mergeCell ref="A280:D280"/>
+    <mergeCell ref="A282:D282"/>
+    <mergeCell ref="A283:D283"/>
+    <mergeCell ref="A309:D309"/>
+    <mergeCell ref="A310:D310"/>
+    <mergeCell ref="A366:D366"/>
+    <mergeCell ref="A316:D316"/>
+    <mergeCell ref="A355:D355"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A159:D159"/>
+    <mergeCell ref="A201:D201"/>
+    <mergeCell ref="A205:D205"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A187:D187"/>
+    <mergeCell ref="A188:D188"/>
+    <mergeCell ref="A192:D192"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A356:D356"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A240:D240"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="A244:D244"/>
+    <mergeCell ref="A246:D246"/>
+    <mergeCell ref="A247:D247"/>
+    <mergeCell ref="A251:D251"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A324:D324"/>
+    <mergeCell ref="A329:D329"/>
+    <mergeCell ref="A339:D339"/>
+    <mergeCell ref="A338:D338"/>
+    <mergeCell ref="A344:D344"/>
+    <mergeCell ref="A290:D290"/>
+    <mergeCell ref="A292:D292"/>
+    <mergeCell ref="A291:D291"/>
+    <mergeCell ref="A295:D295"/>
+    <mergeCell ref="A296:D296"/>
+    <mergeCell ref="A300:D300"/>
+    <mergeCell ref="A301:D301"/>
+    <mergeCell ref="A345:D345"/>
+    <mergeCell ref="A346:D346"/>
+    <mergeCell ref="A387:D387"/>
+    <mergeCell ref="A409:D409"/>
+    <mergeCell ref="A410:D410"/>
+    <mergeCell ref="A415:D415"/>
+    <mergeCell ref="A416:D416"/>
+    <mergeCell ref="A423:D423"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A174:D174"/>
+    <mergeCell ref="A418:D418"/>
+    <mergeCell ref="A354:D354"/>
+    <mergeCell ref="A322:D322"/>
+    <mergeCell ref="A328:D328"/>
+    <mergeCell ref="A303:D303"/>
+    <mergeCell ref="A304:D304"/>
+    <mergeCell ref="A306:D306"/>
+    <mergeCell ref="A305:D305"/>
+    <mergeCell ref="A307:D307"/>
+    <mergeCell ref="A308:D308"/>
+    <mergeCell ref="A357:D357"/>
+    <mergeCell ref="A365:D365"/>
+    <mergeCell ref="A403:D403"/>
+    <mergeCell ref="A404:D404"/>
+    <mergeCell ref="A369:D369"/>
+    <mergeCell ref="A394:D394"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A417:D417"/>
+    <mergeCell ref="A389:D389"/>
+    <mergeCell ref="A286:D286"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A320:D320"/>
+    <mergeCell ref="A321:D321"/>
+    <mergeCell ref="A200:D200"/>
+    <mergeCell ref="A232:D232"/>
+    <mergeCell ref="A233:D233"/>
+    <mergeCell ref="A236:D236"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A259:D259"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A379:D379"/>
+    <mergeCell ref="A380:D380"/>
+    <mergeCell ref="A386:D386"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
@@ -27055,191 +28149,17 @@
     <mergeCell ref="A261:D261"/>
     <mergeCell ref="A393:D393"/>
     <mergeCell ref="A396:D396"/>
-    <mergeCell ref="A394:D394"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A417:D417"/>
-    <mergeCell ref="A389:D389"/>
-    <mergeCell ref="A286:D286"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A320:D320"/>
-    <mergeCell ref="A321:D321"/>
-    <mergeCell ref="A200:D200"/>
-    <mergeCell ref="A232:D232"/>
-    <mergeCell ref="A233:D233"/>
-    <mergeCell ref="A236:D236"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A259:D259"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A379:D379"/>
-    <mergeCell ref="A380:D380"/>
-    <mergeCell ref="A386:D386"/>
-    <mergeCell ref="A387:D387"/>
-    <mergeCell ref="A409:D409"/>
-    <mergeCell ref="A410:D410"/>
-    <mergeCell ref="A415:D415"/>
-    <mergeCell ref="A416:D416"/>
-    <mergeCell ref="A423:D423"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A174:D174"/>
-    <mergeCell ref="A418:D418"/>
-    <mergeCell ref="A354:D354"/>
-    <mergeCell ref="A322:D322"/>
-    <mergeCell ref="A328:D328"/>
-    <mergeCell ref="A303:D303"/>
-    <mergeCell ref="A304:D304"/>
-    <mergeCell ref="A306:D306"/>
-    <mergeCell ref="A305:D305"/>
-    <mergeCell ref="A307:D307"/>
-    <mergeCell ref="A308:D308"/>
-    <mergeCell ref="A357:D357"/>
-    <mergeCell ref="A365:D365"/>
-    <mergeCell ref="A403:D403"/>
-    <mergeCell ref="A404:D404"/>
-    <mergeCell ref="A369:D369"/>
-    <mergeCell ref="A356:D356"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A240:D240"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="A244:D244"/>
-    <mergeCell ref="A246:D246"/>
-    <mergeCell ref="A247:D247"/>
-    <mergeCell ref="A251:D251"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A324:D324"/>
-    <mergeCell ref="A329:D329"/>
-    <mergeCell ref="A339:D339"/>
-    <mergeCell ref="A338:D338"/>
-    <mergeCell ref="A344:D344"/>
-    <mergeCell ref="A290:D290"/>
-    <mergeCell ref="A292:D292"/>
-    <mergeCell ref="A291:D291"/>
-    <mergeCell ref="A295:D295"/>
-    <mergeCell ref="A296:D296"/>
-    <mergeCell ref="A300:D300"/>
-    <mergeCell ref="A301:D301"/>
-    <mergeCell ref="A345:D345"/>
-    <mergeCell ref="A346:D346"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A159:D159"/>
-    <mergeCell ref="A201:D201"/>
-    <mergeCell ref="A205:D205"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="A181:D181"/>
-    <mergeCell ref="A187:D187"/>
-    <mergeCell ref="A188:D188"/>
-    <mergeCell ref="A192:D192"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A388:D388"/>
-    <mergeCell ref="A194:D194"/>
-    <mergeCell ref="A195:D195"/>
-    <mergeCell ref="A215:D215"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A319:D319"/>
-    <mergeCell ref="A272:D272"/>
-    <mergeCell ref="A273:D273"/>
-    <mergeCell ref="A274:D274"/>
-    <mergeCell ref="A279:D279"/>
-    <mergeCell ref="A347:D347"/>
-    <mergeCell ref="A353:D353"/>
-    <mergeCell ref="A325:D325"/>
-    <mergeCell ref="A326:D326"/>
-    <mergeCell ref="A280:D280"/>
-    <mergeCell ref="A282:D282"/>
-    <mergeCell ref="A283:D283"/>
-    <mergeCell ref="A309:D309"/>
-    <mergeCell ref="A310:D310"/>
-    <mergeCell ref="A366:D366"/>
-    <mergeCell ref="A316:D316"/>
-    <mergeCell ref="A355:D355"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A165:D165"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A160:D160"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A391:D391"/>
-    <mergeCell ref="A262:D262"/>
-    <mergeCell ref="A235:D235"/>
-    <mergeCell ref="A202:D202"/>
-    <mergeCell ref="A168:D168"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A317:D317"/>
-    <mergeCell ref="A318:D318"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A224:D224"/>
-    <mergeCell ref="A226:D226"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A289:D289"/>
-    <mergeCell ref="A323:D323"/>
-    <mergeCell ref="A358:D358"/>
-    <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A268:D268"/>
-    <mergeCell ref="A269:D269"/>
-    <mergeCell ref="A271:D271"/>
-    <mergeCell ref="A206:D206"/>
-    <mergeCell ref="A210:D210"/>
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="A288:D288"/>
-    <mergeCell ref="A211:D211"/>
-    <mergeCell ref="A212:D212"/>
-    <mergeCell ref="A213:D213"/>
-    <mergeCell ref="A214:D214"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <conditionalFormatting sqref="M32:T32 M56:T77 M79:T104 M201:T232 M234:T259 M261:T286 M288:T320 M390:T1048576 M48:T48 M53:T54 M14:T14 M29:T29 M322:T355 M143:T165 M357:T388 M167:T199 M16:T23 Q15:T15 M34:T45 M106:T141">
     <cfRule type="cellIs" dxfId="175" priority="269" operator="equal">
@@ -27655,7 +28575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87786A15-F039-4732-8224-D8AE4342938B}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>

</xml_diff>